<commit_message>
Option pricing working in excel
</commit_message>
<xml_diff>
--- a/ExampleSpreadsheet/ICE Brent Options - Fixed Inputs.xlsx
+++ b/ExampleSpreadsheet/ICE Brent Options - Fixed Inputs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="12405" tabRatio="708" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="12405" tabRatio="708" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LCO Vol Surf" sheetId="1" r:id="rId1"/>
@@ -332,13 +332,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
-    <numFmt numFmtId="167" formatCode="&quot;R&quot;#,##0.0,,&quot;M&quot;_);[Red]\(&quot;R&quot;#,##0.0,,&quot;M&quot;\)"/>
-    <numFmt numFmtId="168" formatCode="\ \ @"/>
-    <numFmt numFmtId="169" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="168" formatCode="&quot;R&quot;#,##0.0,,&quot;M&quot;_);[Red]\(&quot;R&quot;#,##0.0,,&quot;M&quot;\)"/>
+    <numFmt numFmtId="169" formatCode="\ \ @"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0.0000_ ;_ * \-#,##0.0000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -858,12 +858,12 @@
   </borders>
   <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="8" fillId="4" borderId="0">
@@ -873,7 +873,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="37" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -917,18 +917,18 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
@@ -938,7 +938,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -955,7 +955,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -966,7 +966,7 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -990,20 +990,20 @@
     <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="36" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1022,12 +1022,12 @@
     <xf numFmtId="10" fontId="4" fillId="37" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="37" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="4" fillId="37" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="37" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="37" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="37" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="57">
     <cellStyle name="$M" xfId="6"/>
@@ -3307,7 +3307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4489,11 +4489,11 @@
   <sheetPr codeName="Sheet20">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T39"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="12.75"/>
@@ -5965,7 +5965,7 @@
     <row r="2" spans="1:20">
       <c r="B2" s="48">
         <f>J2/H2</f>
-        <v>1.7662770449645817</v>
+        <v>1.7662328205052362</v>
       </c>
       <c r="C2" s="30">
         <v>42947</v>
@@ -5991,22 +5991,22 @@
       </c>
       <c r="J2" s="20">
         <f t="shared" ref="J2:J7" si="0">T2</f>
-        <v>17662.770449645817</v>
+        <v>17662.328205052363</v>
       </c>
       <c r="K2" s="34">
-        <f>_xll.XLLBlackDelta(D2,N2,G2,O2,M2*SQRT(O2/365),1)</f>
-        <v>-0.27011166969869649</v>
+        <f>_xll.xllBlackDelta(D2,N2,G2,O2,M2*SQRT(O2/365),1)</f>
+        <v>-0.27010976321434743</v>
       </c>
       <c r="L2" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D2,N2,G2,O2,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.31741071276495109</v>
+        <f>_xll.xllBlackVolOffSurface(D2,N2,G2,O2,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.31740638936155174</v>
       </c>
       <c r="M2" s="35">
         <f>L2</f>
-        <v>0.31741071276495109</v>
+        <v>0.31740638936155174</v>
       </c>
       <c r="N2" s="36">
-        <f>_xll.XLLInterpolate(C2,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C2,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O2" s="31">
@@ -6018,7 +6018,7 @@
         <v>130</v>
       </c>
       <c r="Q2" s="37">
-        <f>_xll.XLLInterpolate(P2,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P2,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R2" s="37">
@@ -6026,22 +6026,22 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S2" s="38">
-        <f>_xll.XLLBlack(D2,N2,G2,O2,M2*SQRT(O2/365),1)*H2</f>
-        <v>17738.413117637996</v>
+        <f>_xll.xllBlack(D2,N2,G2,O2,M2*SQRT(O2/365),1)*H2</f>
+        <v>17737.968979085661</v>
       </c>
       <c r="T2" s="39">
         <f t="shared" ref="T2:T7" si="2">S2*R2</f>
-        <v>17662.770449645817</v>
+        <v>17662.328205052363</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="48">
         <f>AVERAGE(B2:B4)</f>
-        <v>2.080903357995004</v>
+        <v>2.0810087329266431</v>
       </c>
       <c r="B3" s="48">
         <f t="shared" ref="B3:B13" si="3">J3/H3</f>
-        <v>2.1027013841668469</v>
+        <v>2.1030879788711618</v>
       </c>
       <c r="C3" s="30">
         <v>42978</v>
@@ -6071,22 +6071,22 @@
       </c>
       <c r="J3" s="20">
         <f t="shared" si="0"/>
-        <v>21027.013841668468</v>
+        <v>21030.879788711616</v>
       </c>
       <c r="K3" s="34">
-        <f>_xll.XLLBlackDelta(D3,N3,G3,O3,M3*SQRT(O3/365),1)</f>
-        <v>-0.2820556381911119</v>
+        <f>_xll.xllBlackDelta(D3,N3,G3,O3,M3*SQRT(O3/365),1)</f>
+        <v>-0.28206908288853993</v>
       </c>
       <c r="L3" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D3,N3,G3,O3,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.31474521578550424</v>
+        <f>_xll.xllBlackVolOffSurface(D3,N3,G3,O3,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.31477880660800961</v>
       </c>
       <c r="M3" s="35">
         <f t="shared" ref="M3:M4" si="7">L3</f>
-        <v>0.31474521578550424</v>
+        <v>0.31477880660800961</v>
       </c>
       <c r="N3" s="36">
-        <f>_xll.XLLInterpolate(C3,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C3,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O3" s="31">
@@ -6098,7 +6098,7 @@
         <v>161</v>
       </c>
       <c r="Q3" s="37">
-        <f>_xll.XLLInterpolate(P3,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P3,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R3" s="37">
@@ -6106,18 +6106,18 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S3" s="38">
-        <f>_xll.XLLBlack(D3,N3,G3,O3,M3*SQRT(O3/365),1)*H3</f>
-        <v>21141.05622850934</v>
+        <f>_xll.xllBlack(D3,N3,G3,O3,M3*SQRT(O3/365),1)*H3</f>
+        <v>21144.943142953351</v>
       </c>
       <c r="T3" s="39">
         <f t="shared" si="2"/>
-        <v>21027.013841668468</v>
+        <v>21030.879788711616</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" s="48">
         <f t="shared" si="3"/>
-        <v>2.3737316448535832</v>
+        <v>2.3737053994035318</v>
       </c>
       <c r="C4" s="30">
         <v>43007</v>
@@ -6147,22 +6147,22 @@
       </c>
       <c r="J4" s="20">
         <f t="shared" si="0"/>
-        <v>23737.316448535832</v>
+        <v>23737.053994035319</v>
       </c>
       <c r="K4" s="34">
-        <f>_xll.XLLBlackDelta(D4,N4,G4,O4,M4*SQRT(O4/365),1)</f>
-        <v>-0.29026372294806191</v>
+        <f>_xll.xllBlackDelta(D4,N4,G4,O4,M4*SQRT(O4/365),1)</f>
+        <v>-0.29026303702914058</v>
       </c>
       <c r="L4" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D4,N4,G4,O4,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.31077037253582623</v>
+        <f>_xll.xllBlackVolOffSurface(D4,N4,G4,O4,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.31076843555617095</v>
       </c>
       <c r="M4" s="35">
         <f t="shared" si="7"/>
-        <v>0.31077037253582623</v>
+        <v>0.31076843555617095</v>
       </c>
       <c r="N4" s="36">
-        <f>_xll.XLLInterpolate(C4,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C4,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O4" s="31">
@@ -6174,7 +6174,7 @@
         <v>190</v>
       </c>
       <c r="Q4" s="37">
-        <f>_xll.XLLInterpolate(P4,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P4,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R4" s="37">
@@ -6182,19 +6182,19 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S4" s="38">
-        <f>_xll.XLLBlack(D4,N4,G4,O4,M4*SQRT(O4/365),1)*H4</f>
-        <v>23892.376276573108</v>
+        <f>_xll.xllBlack(D4,N4,G4,O4,M4*SQRT(O4/365),1)*H4</f>
+        <v>23892.112107634915</v>
       </c>
       <c r="T4" s="39">
         <f t="shared" si="2"/>
-        <v>23737.316448535832</v>
+        <v>23737.053994035319</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="58" customFormat="1">
       <c r="A5" s="49"/>
       <c r="B5" s="49">
         <f t="shared" si="3"/>
-        <v>2.8119843303279701</v>
+        <v>2.8123745184598841</v>
       </c>
       <c r="C5" s="50">
         <v>43039</v>
@@ -6224,22 +6224,22 @@
       </c>
       <c r="J5" s="54">
         <f t="shared" si="0"/>
-        <v>28119.8433032797</v>
+        <v>28123.74518459884</v>
       </c>
       <c r="K5" s="55">
-        <f>_xll.XLLBlackDelta(D5,N5,G5,O5,M5*SQRT(O5/365),1)</f>
-        <v>-0.30210106080103594</v>
+        <f>_xll.xllBlackDelta(D5,N5,G5,O5,M5*SQRT(O5/365),1)</f>
+        <v>-0.30210950670851022</v>
       </c>
       <c r="L5" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D5,N5,G5,O5,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.30754674515840547</v>
+        <f>_xll.xllBlackVolOffSurface(D5,N5,G5,O5,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.30757466920776261</v>
       </c>
       <c r="M5" s="35">
         <f>L5+0.01</f>
-        <v>0.31754674515840547</v>
+        <v>0.31757466920776262</v>
       </c>
       <c r="N5" s="36">
-        <f>_xll.XLLInterpolate(C5,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C5,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O5" s="51">
@@ -6251,7 +6251,7 @@
         <v>222</v>
       </c>
       <c r="Q5" s="56">
-        <f>_xll.XLLInterpolate(P5,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P5,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R5" s="56">
@@ -6259,22 +6259,22 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S5" s="38">
-        <f>_xll.XLLBlack(D5,N5,G5,O5,M5*SQRT(O5/365),1)*H5</f>
-        <v>28339.040018117015</v>
+        <f>_xll.xllBlack(D5,N5,G5,O5,M5*SQRT(O5/365),1)*H5</f>
+        <v>28342.972314952971</v>
       </c>
       <c r="T5" s="57">
         <f t="shared" si="2"/>
-        <v>28119.8433032797</v>
+        <v>28123.74518459884</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="58" customFormat="1">
       <c r="A6" s="49">
         <f>AVERAGE(B5:B7)</f>
-        <v>2.9869025620816516</v>
+        <v>2.9872364235796929</v>
       </c>
       <c r="B6" s="49">
         <f t="shared" si="3"/>
-        <v>2.9920604391692214</v>
+        <v>2.9923712566763121</v>
       </c>
       <c r="C6" s="50">
         <v>43069</v>
@@ -6304,22 +6304,22 @@
       </c>
       <c r="J6" s="54">
         <f t="shared" si="0"/>
-        <v>29920.604391692214</v>
+        <v>29923.712566763119</v>
       </c>
       <c r="K6" s="55">
-        <f>_xll.XLLBlackDelta(D6,N6,G6,O6,M6*SQRT(O6/365),1)</f>
-        <v>-0.30582259099492082</v>
+        <f>_xll.xllBlackDelta(D6,N6,G6,O6,M6*SQRT(O6/365),1)</f>
+        <v>-0.30582858935894086</v>
       </c>
       <c r="L6" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D6,N6,G6,O6,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29969137337425855</v>
+        <f>_xll.xllBlackVolOffSurface(D6,N6,G6,O6,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.2997121519969963</v>
       </c>
       <c r="M6" s="35">
         <f>L6+0.01</f>
-        <v>0.30969137337425856</v>
+        <v>0.30971215199699631</v>
       </c>
       <c r="N6" s="36">
-        <f>_xll.XLLInterpolate(C6,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C6,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O6" s="51">
@@ -6331,7 +6331,7 @@
         <v>252</v>
       </c>
       <c r="Q6" s="56">
-        <f>_xll.XLLInterpolate(P6,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P6,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R6" s="56">
@@ -6339,19 +6339,19 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S6" s="38">
-        <f>_xll.XLLBlack(D6,N6,G6,O6,M6*SQRT(O6/365),1)*H6</f>
-        <v>30190.543767334253</v>
+        <f>_xll.xllBlack(D6,N6,G6,O6,M6*SQRT(O6/365),1)*H6</f>
+        <v>30193.679983912178</v>
       </c>
       <c r="T6" s="57">
         <f t="shared" si="2"/>
-        <v>29920.604391692214</v>
+        <v>29923.712566763119</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="58" customFormat="1">
       <c r="A7" s="49"/>
       <c r="B7" s="49">
         <f t="shared" si="3"/>
-        <v>3.1566629167477638</v>
+        <v>3.1569634956028829</v>
       </c>
       <c r="C7" s="50">
         <v>43097</v>
@@ -6381,22 +6381,22 @@
       </c>
       <c r="J7" s="54">
         <f t="shared" si="0"/>
-        <v>31566.629167477637</v>
+        <v>31569.634956028829</v>
       </c>
       <c r="K7" s="55">
-        <f>_xll.XLLBlackDelta(D7,N7,G7,O7,M7*SQRT(O7/365),1)</f>
-        <v>-0.30927510372135725</v>
+        <f>_xll.xllBlackDelta(D7,N7,G7,O7,M7*SQRT(O7/365),1)</f>
+        <v>-0.30928030961832054</v>
       </c>
       <c r="L7" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D7,N7,G7,O7,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29357155121085898</v>
+        <f>_xll.xllBlackVolOffSurface(D7,N7,G7,O7,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.29359052557809928</v>
       </c>
       <c r="M7" s="35">
         <f>L7+0.01</f>
-        <v>0.30357155121085899</v>
+        <v>0.30359052557809929</v>
       </c>
       <c r="N7" s="36">
-        <f>_xll.XLLInterpolate(C7,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C7,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O7" s="51">
@@ -6408,7 +6408,7 @@
         <v>281</v>
       </c>
       <c r="Q7" s="56">
-        <f>_xll.XLLInterpolate(P7,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P7,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R7" s="56">
@@ -6416,18 +6416,18 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S7" s="38">
-        <f>_xll.XLLBlack(D7,N7,G7,O7,M7*SQRT(O7/365),1)*H7</f>
-        <v>31890.079225080506</v>
+        <f>_xll.xllBlack(D7,N7,G7,O7,M7*SQRT(O7/365),1)*H7</f>
+        <v>31893.115812690881</v>
       </c>
       <c r="T7" s="57">
         <f t="shared" si="2"/>
-        <v>31566.629167477637</v>
+        <v>31569.634956028829</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="B8" s="48">
         <f t="shared" si="3"/>
-        <v>3.5513313062586951</v>
+        <v>3.5516766330417231</v>
       </c>
       <c r="C8" s="30">
         <v>43131</v>
@@ -6457,22 +6457,22 @@
       </c>
       <c r="J8" s="20">
         <f t="shared" ref="J8" si="13">T8</f>
-        <v>35513.313062586953</v>
+        <v>35516.766330417231</v>
       </c>
       <c r="K8" s="34">
-        <f>_xll.XLLBlackDelta(D8,N8,G8,O8,M8*SQRT(O8/365),1)</f>
-        <v>-0.31688449011533426</v>
+        <f>_xll.xllBlackDelta(D8,N8,G8,O8,M8*SQRT(O8/365),1)</f>
+        <v>-0.31688906422406737</v>
       </c>
       <c r="L8" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D8,N8,G8,O8,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28833497668183233</v>
+        <f>_xll.xllBlackVolOffSurface(D8,N8,G8,O8,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28835534081549791</v>
       </c>
       <c r="M8" s="35">
         <f>L8+0.02</f>
-        <v>0.30833497668183235</v>
+        <v>0.30835534081549792</v>
       </c>
       <c r="N8" s="36">
-        <f>_xll.XLLInterpolate(C8,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C8,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O8" s="31">
@@ -6484,7 +6484,7 @@
         <v>314</v>
       </c>
       <c r="Q8" s="37">
-        <f>_xll.XLLInterpolate(P8,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P8,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R8" s="37">
@@ -6492,22 +6492,22 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S8" s="38">
-        <f>_xll.XLLBlack(D8,N8,G8,O8,M8*SQRT(O8/365),1)*H8</f>
-        <v>35927.914383963434</v>
+        <f>_xll.xllBlack(D8,N8,G8,O8,M8*SQRT(O8/365),1)*H8</f>
+        <v>35931.407967080631</v>
       </c>
       <c r="T8" s="39">
         <f t="shared" ref="T8" si="15">S8*R8</f>
-        <v>35513.313062586953</v>
+        <v>35516.766330417231</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="48">
         <f>AVERAGE(B8:B10)</f>
-        <v>3.7239096145546409</v>
+        <v>3.7241097438515567</v>
       </c>
       <c r="B9" s="48">
         <f t="shared" si="3"/>
-        <v>3.7265749071511105</v>
+        <v>3.7267211921408148</v>
       </c>
       <c r="C9" s="30">
         <v>43159</v>
@@ -6537,22 +6537,22 @@
       </c>
       <c r="J9" s="20">
         <f t="shared" ref="J9:J13" si="17">T9</f>
-        <v>37265.749071511105</v>
+        <v>37267.211921408147</v>
       </c>
       <c r="K9" s="34">
-        <f>_xll.XLLBlackDelta(D9,N9,G9,O9,M9*SQRT(O9/365),1)</f>
-        <v>-0.31989149387805216</v>
+        <f>_xll.xllBlackDelta(D9,N9,G9,O9,M9*SQRT(O9/365),1)</f>
+        <v>-0.31989322539653475</v>
       </c>
       <c r="L9" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D9,N9,G9,O9,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28455075980492628</v>
+        <f>_xll.xllBlackVolOffSurface(D9,N9,G9,O9,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28455903816319966</v>
       </c>
       <c r="M9" s="35">
         <f>L9+0.02</f>
-        <v>0.3045507598049263</v>
+        <v>0.30455903816319968</v>
       </c>
       <c r="N9" s="36">
-        <f>_xll.XLLInterpolate(C9,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C9,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O9" s="31">
@@ -6564,7 +6564,7 @@
         <v>342</v>
       </c>
       <c r="Q9" s="37">
-        <f>_xll.XLLInterpolate(P9,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P9,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R9" s="37">
@@ -6572,18 +6572,18 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S9" s="38">
-        <f>_xll.XLLBlack(D9,N9,G9,O9,M9*SQRT(O9/365),1)*H9</f>
-        <v>37747.356802190414</v>
+        <f>_xll.xllBlack(D9,N9,G9,O9,M9*SQRT(O9/365),1)*H9</f>
+        <v>37748.838557378156</v>
       </c>
       <c r="T9" s="39">
         <f t="shared" ref="T9:T13" si="19">S9*R9</f>
-        <v>37265.749071511105</v>
+        <v>37267.211921408147</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="B10" s="48">
         <f t="shared" si="3"/>
-        <v>3.8938226302541175</v>
+        <v>3.8939314063721322</v>
       </c>
       <c r="C10" s="30">
         <v>43188</v>
@@ -6613,22 +6613,22 @@
       </c>
       <c r="J10" s="20">
         <f t="shared" si="17"/>
-        <v>38938.226302541174</v>
+        <v>38939.314063721322</v>
       </c>
       <c r="K10" s="34">
-        <f>_xll.XLLBlackDelta(D10,N10,G10,O10,M10*SQRT(O10/365),1)</f>
-        <v>-0.3227492483050769</v>
+        <f>_xll.xllBlackDelta(D10,N10,G10,O10,M10*SQRT(O10/365),1)</f>
+        <v>-0.32275039161764552</v>
       </c>
       <c r="L10" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D10,N10,G10,O10,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28058381281862099</v>
+        <f>_xll.xllBlackVolOffSurface(D10,N10,G10,O10,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28058971047977793</v>
       </c>
       <c r="M10" s="35">
         <f>L10+0.02</f>
-        <v>0.30058381281862101</v>
+        <v>0.30058971047977795</v>
       </c>
       <c r="N10" s="36">
-        <f>_xll.XLLInterpolate(C10,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C10,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O10" s="31">
@@ -6640,7 +6640,7 @@
         <v>372</v>
       </c>
       <c r="Q10" s="37">
-        <f>_xll.XLLInterpolate(P10,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P10,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R10" s="37">
@@ -6648,19 +6648,19 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S10" s="38">
-        <f>_xll.XLLBlack(D10,N10,G10,O10,M10*SQRT(O10/365),1)*H10</f>
-        <v>39494.970594135455</v>
+        <f>_xll.xllBlack(D10,N10,G10,O10,M10*SQRT(O10/365),1)*H10</f>
+        <v>39496.073908279497</v>
       </c>
       <c r="T10" s="39">
         <f t="shared" si="19"/>
-        <v>38938.226302541174</v>
+        <v>38939.314063721322</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="58" customFormat="1">
       <c r="A11" s="49"/>
       <c r="B11" s="49">
         <f t="shared" si="3"/>
-        <v>4.208352440596264</v>
+        <v>4.2084301804314075</v>
       </c>
       <c r="C11" s="50">
         <v>43220</v>
@@ -6690,22 +6690,22 @@
       </c>
       <c r="J11" s="54">
         <f t="shared" si="17"/>
-        <v>42083.524405962642</v>
+        <v>42084.301804314076</v>
       </c>
       <c r="K11" s="55">
-        <f>_xll.XLLBlackDelta(D11,N11,G11,O11,M11*SQRT(O11/365),1)</f>
-        <v>-0.32797977186047689</v>
+        <f>_xll.xllBlackDelta(D11,N11,G11,O11,M11*SQRT(O11/365),1)</f>
+        <v>-0.3279804101698518</v>
       </c>
       <c r="L11" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D11,N11,G11,O11,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27767586961246593</v>
+        <f>_xll.xllBlackVolOffSurface(D11,N11,G11,O11,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27767987513460557</v>
       </c>
       <c r="M11" s="35">
         <f>L11+0.025</f>
-        <v>0.30267586961246595</v>
+        <v>0.30267987513460559</v>
       </c>
       <c r="N11" s="36">
-        <f>_xll.XLLInterpolate(C11,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C11,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O11" s="51">
@@ -6717,7 +6717,7 @@
         <v>403</v>
       </c>
       <c r="Q11" s="56">
-        <f>_xll.XLLInterpolate(P11,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P11,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R11" s="56">
@@ -6725,22 +6725,22 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S11" s="38">
-        <f>_xll.XLLBlack(D11,N11,G11,O11,M11*SQRT(O11/365),1)*H11</f>
-        <v>42745.881523049538</v>
+        <f>_xll.xllBlack(D11,N11,G11,O11,M11*SQRT(O11/365),1)*H11</f>
+        <v>42746.671156957244</v>
       </c>
       <c r="T11" s="57">
         <f t="shared" si="19"/>
-        <v>42083.524405962642</v>
+        <v>42084.301804314076</v>
       </c>
     </row>
     <row r="12" spans="1:20" s="58" customFormat="1">
       <c r="A12" s="49">
         <f>AVERAGE(B11:B13)</f>
-        <v>4.3832026088708469</v>
+        <v>4.3833292980584817</v>
       </c>
       <c r="B12" s="49">
         <f t="shared" si="3"/>
-        <v>4.3875730709498679</v>
+        <v>4.3878267323519289</v>
       </c>
       <c r="C12" s="50">
         <v>43251</v>
@@ -6770,22 +6770,22 @@
       </c>
       <c r="J12" s="54">
         <f t="shared" si="17"/>
-        <v>43875.730709498683</v>
+        <v>43878.267323519292</v>
       </c>
       <c r="K12" s="55">
-        <f>_xll.XLLBlackDelta(D12,N12,G12,O12,M12*SQRT(O12/365),1)</f>
-        <v>-0.3303109382661793</v>
+        <f>_xll.xllBlackDelta(D12,N12,G12,O12,M12*SQRT(O12/365),1)</f>
+        <v>-0.33031268997619689</v>
       </c>
       <c r="L12" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D12,N12,G12,O12,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27485254392406788</v>
+        <f>_xll.xllBlackVolOffSurface(D12,N12,G12,O12,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27486507531972315</v>
       </c>
       <c r="M12" s="35">
         <f>L12+0.025</f>
-        <v>0.2998525439240679</v>
+        <v>0.29986507531972317</v>
       </c>
       <c r="N12" s="36">
-        <f>_xll.XLLInterpolate(C12,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C12,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O12" s="51">
@@ -6797,7 +6797,7 @@
         <v>434</v>
       </c>
       <c r="Q12" s="56">
-        <f>_xll.XLLInterpolate(P12,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P12,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R12" s="56">
@@ -6805,19 +6805,19 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S12" s="38">
-        <f>_xll.XLLBlack(D12,N12,G12,O12,M12*SQRT(O12/365),1)*H12</f>
-        <v>44631.230730047449</v>
+        <f>_xll.xllBlack(D12,N12,G12,O12,M12*SQRT(O12/365),1)*H12</f>
+        <v>44633.811022245347</v>
       </c>
       <c r="T12" s="57">
         <f t="shared" si="19"/>
-        <v>43875.730709498683</v>
+        <v>43878.267323519292</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="58" customFormat="1">
       <c r="A13" s="49"/>
       <c r="B13" s="49">
         <f t="shared" si="3"/>
-        <v>4.5536823150664096</v>
+        <v>4.5537309813921087</v>
       </c>
       <c r="C13" s="50">
         <v>43280</v>
@@ -6847,22 +6847,22 @@
       </c>
       <c r="J13" s="54">
         <f t="shared" si="17"/>
-        <v>45536.823150664095</v>
+        <v>45537.309813921085</v>
       </c>
       <c r="K13" s="55">
-        <f>_xll.XLLBlackDelta(D13,N13,G13,O13,M13*SQRT(O13/365),1)</f>
-        <v>-0.33254471547844533</v>
+        <f>_xll.xllBlackDelta(D13,N13,G13,O13,M13*SQRT(O13/365),1)</f>
+        <v>-0.33254501125760916</v>
       </c>
       <c r="L13" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D13,N13,G13,O13,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27247081730796219</v>
+        <f>_xll.xllBlackVolOffSurface(D13,N13,G13,O13,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27247311737224561</v>
       </c>
       <c r="M13" s="35">
         <f>L13+0.025</f>
-        <v>0.29747081730796221</v>
+        <v>0.29747311737224563</v>
       </c>
       <c r="N13" s="36">
-        <f>_xll.XLLInterpolate(C13,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C13,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O13" s="51">
@@ -6874,7 +6874,7 @@
         <v>463</v>
       </c>
       <c r="Q13" s="56">
-        <f>_xll.XLLInterpolate(P13,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P13,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R13" s="56">
@@ -6882,18 +6882,18 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S13" s="38">
-        <f>_xll.XLLBlack(D13,N13,G13,O13,M13*SQRT(O13/365),1)*H13</f>
-        <v>46385.595508153056</v>
+        <f>_xll.xllBlack(D13,N13,G13,O13,M13*SQRT(O13/365),1)*H13</f>
+        <v>46386.091242449511</v>
       </c>
       <c r="T13" s="57">
         <f t="shared" si="19"/>
-        <v>45536.823150664095</v>
+        <v>45537.309813921085</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="B15" s="48">
         <f>J15/H15</f>
-        <v>2.4164943142680317</v>
+        <v>2.4164889260678812</v>
       </c>
       <c r="C15" s="30">
         <v>42947</v>
@@ -6919,22 +6919,22 @@
       </c>
       <c r="J15" s="20">
         <f t="shared" ref="J15:J26" si="24">T15</f>
-        <v>24164.943142680317</v>
+        <v>24164.88926067881</v>
       </c>
       <c r="K15" s="34">
-        <f>_xll.XLLBlackDelta(D15,N15,G15,O15,M15*SQRT(O15/365),1)</f>
-        <v>-0.3457380608595747</v>
+        <f>_xll.xllBlackDelta(D15,N15,G15,O15,M15*SQRT(O15/365),1)</f>
+        <v>-0.34573797134889972</v>
       </c>
       <c r="L15" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D15,N15,G15,O15,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.3086691951515862</v>
+        <f>_xll.xllBlackVolOffSurface(D15,N15,G15,O15,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.3086688231518766</v>
       </c>
       <c r="M15" s="35">
         <f>L15</f>
-        <v>0.3086691951515862</v>
+        <v>0.3086688231518766</v>
       </c>
       <c r="N15" s="36">
-        <f>_xll.XLLInterpolate(C15,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C15,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O15" s="31">
@@ -6946,7 +6946,7 @@
         <v>130</v>
       </c>
       <c r="Q15" s="37">
-        <f>_xll.XLLInterpolate(P15,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P15,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R15" s="37">
@@ -6954,22 +6954,22 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S15" s="38">
-        <f>_xll.XLLBlack(D15,N15,G15,O15,M15*SQRT(O15/365),1)*H15</f>
-        <v>24268.43204757226</v>
+        <f>_xll.xllBlack(D15,N15,G15,O15,M15*SQRT(O15/365),1)*H15</f>
+        <v>24268.377934815428</v>
       </c>
       <c r="T15" s="39">
         <f t="shared" ref="T15:T26" si="26">S15*R15</f>
-        <v>24164.943142680317</v>
+        <v>24164.88926067881</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="48">
         <f>AVERAGE(B15:B17)</f>
-        <v>2.7608729866463975</v>
+        <v>2.7610811646590285</v>
       </c>
       <c r="B16" s="48">
         <f t="shared" ref="B16:B26" si="27">J16/H16</f>
-        <v>2.7852315008743118</v>
+        <v>2.7857861311981327</v>
       </c>
       <c r="C16" s="30">
         <v>42978</v>
@@ -6999,22 +6999,22 @@
       </c>
       <c r="J16" s="20">
         <f t="shared" si="24"/>
-        <v>27852.315008743117</v>
+        <v>27857.861311981327</v>
       </c>
       <c r="K16" s="34">
-        <f>_xll.XLLBlackDelta(D16,N16,G16,O16,M16*SQRT(O16/365),1)</f>
-        <v>-0.35140043542323518</v>
+        <f>_xll.xllBlackDelta(D16,N16,G16,O16,M16*SQRT(O16/365),1)</f>
+        <v>-0.35141008466071144</v>
       </c>
       <c r="L16" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D16,N16,G16,O16,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.30691254050033739</v>
+        <f>_xll.xllBlackVolOffSurface(D16,N16,G16,O16,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.30695635331106219</v>
       </c>
       <c r="M16" s="35">
         <f t="shared" ref="M16:M17" si="30">L16</f>
-        <v>0.30691254050033739</v>
+        <v>0.30695635331106219</v>
       </c>
       <c r="N16" s="36">
-        <f>_xll.XLLInterpolate(C16,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C16,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O16" s="31">
@@ -7026,7 +7026,7 @@
         <v>161</v>
       </c>
       <c r="Q16" s="37">
-        <f>_xll.XLLInterpolate(P16,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P16,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R16" s="37">
@@ -7034,18 +7034,18 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S16" s="38">
-        <f>_xll.XLLBlack(D16,N16,G16,O16,M16*SQRT(O16/365),1)*H16</f>
-        <v>28003.375188118014</v>
+        <f>_xll.xllBlack(D16,N16,G16,O16,M16*SQRT(O16/365),1)*H16</f>
+        <v>28008.951572358888</v>
       </c>
       <c r="T16" s="39">
         <f t="shared" si="26"/>
-        <v>27852.315008743117</v>
+        <v>27857.861311981327</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="B17" s="48">
         <f t="shared" si="27"/>
-        <v>3.0808931447968497</v>
+        <v>3.0809684367110712</v>
       </c>
       <c r="C17" s="30">
         <v>43007</v>
@@ -7075,22 +7075,22 @@
       </c>
       <c r="J17" s="20">
         <f t="shared" si="24"/>
-        <v>30808.931447968498</v>
+        <v>30809.684367110713</v>
       </c>
       <c r="K17" s="34">
-        <f>_xll.XLLBlackDelta(D17,N17,G17,O17,M17*SQRT(O17/365),1)</f>
-        <v>-0.35546428340615044</v>
+        <f>_xll.xllBlackDelta(D17,N17,G17,O17,M17*SQRT(O17/365),1)</f>
+        <v>-0.35546532307734779</v>
       </c>
       <c r="L17" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D17,N17,G17,O17,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.30364802993304857</v>
+        <f>_xll.xllBlackVolOffSurface(D17,N17,G17,O17,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.30365346769227924</v>
       </c>
       <c r="M17" s="35">
         <f t="shared" si="30"/>
-        <v>0.30364802993304857</v>
+        <v>0.30365346769227924</v>
       </c>
       <c r="N17" s="36">
-        <f>_xll.XLLInterpolate(C17,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C17,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O17" s="31">
@@ -7102,7 +7102,7 @@
         <v>190</v>
       </c>
       <c r="Q17" s="37">
-        <f>_xll.XLLInterpolate(P17,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P17,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R17" s="37">
@@ -7110,19 +7110,19 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S17" s="38">
-        <f>_xll.XLLBlack(D17,N17,G17,O17,M17*SQRT(O17/365),1)*H17</f>
-        <v>31010.185352245826</v>
+        <f>_xll.xllBlack(D17,N17,G17,O17,M17*SQRT(O17/365),1)*H17</f>
+        <v>31010.943189699381</v>
       </c>
       <c r="T17" s="39">
         <f t="shared" si="26"/>
-        <v>30808.931447968498</v>
+        <v>30809.684367110713</v>
       </c>
     </row>
     <row r="18" spans="1:20" s="58" customFormat="1">
       <c r="A18" s="49"/>
       <c r="B18" s="49">
         <f t="shared" si="27"/>
-        <v>3.5537898136202291</v>
+        <v>3.5542670900299278</v>
       </c>
       <c r="C18" s="50">
         <v>43039</v>
@@ -7152,22 +7152,22 @@
       </c>
       <c r="J18" s="54">
         <f t="shared" si="24"/>
-        <v>35537.89813620229</v>
+        <v>35542.670900299279</v>
       </c>
       <c r="K18" s="55">
-        <f>_xll.XLLBlackDelta(D18,N18,G18,O18,M18*SQRT(O18/365),1)</f>
-        <v>-0.36195990320188931</v>
+        <f>_xll.xllBlackDelta(D18,N18,G18,O18,M18*SQRT(O18/365),1)</f>
+        <v>-0.36196426169418083</v>
       </c>
       <c r="L18" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D18,N18,G18,O18,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.30086723662567505</v>
+        <f>_xll.xllBlackVolOffSurface(D18,N18,G18,O18,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.30089879007099096</v>
       </c>
       <c r="M18" s="35">
         <f>L18+0.01</f>
-        <v>0.31086723662567506</v>
+        <v>0.31089879007099097</v>
       </c>
       <c r="N18" s="36">
-        <f>_xll.XLLInterpolate(C18,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C18,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O18" s="51">
@@ -7179,7 +7179,7 @@
         <v>222</v>
       </c>
       <c r="Q18" s="56">
-        <f>_xll.XLLInterpolate(P18,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P18,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R18" s="56">
@@ -7187,22 +7187,22 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S18" s="38">
-        <f>_xll.XLLBlack(D18,N18,G18,O18,M18*SQRT(O18/365),1)*H18</f>
-        <v>35814.919257538699</v>
+        <f>_xll.xllBlack(D18,N18,G18,O18,M18*SQRT(O18/365),1)*H18</f>
+        <v>35819.729225762312</v>
       </c>
       <c r="T18" s="57">
         <f t="shared" si="26"/>
-        <v>35537.89813620229</v>
+        <v>35542.670900299279</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="58" customFormat="1">
       <c r="A19" s="49">
         <f>AVERAGE(B18:B20)</f>
-        <v>3.7453913055293544</v>
+        <v>3.7457932339052555</v>
       </c>
       <c r="B19" s="49">
         <f t="shared" si="27"/>
-        <v>3.7520866440894833</v>
+        <v>3.7524648723895009</v>
       </c>
       <c r="C19" s="50">
         <v>43069</v>
@@ -7232,22 +7232,22 @@
       </c>
       <c r="J19" s="54">
         <f t="shared" si="24"/>
-        <v>37520.866440894832</v>
+        <v>37524.648723895007</v>
       </c>
       <c r="K19" s="55">
-        <f>_xll.XLLBlackDelta(D19,N19,G19,O19,M19*SQRT(O19/365),1)</f>
-        <v>-0.36366084086971773</v>
+        <f>_xll.xllBlackDelta(D19,N19,G19,O19,M19*SQRT(O19/365),1)</f>
+        <v>-0.36366372008794157</v>
       </c>
       <c r="L19" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D19,N19,G19,O19,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29379551832588913</v>
+        <f>_xll.xllBlackVolOffSurface(D19,N19,G19,O19,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.29381889318776599</v>
       </c>
       <c r="M19" s="35">
         <f>L19+0.01</f>
-        <v>0.30379551832588914</v>
+        <v>0.303818893187766</v>
       </c>
       <c r="N19" s="36">
-        <f>_xll.XLLInterpolate(C19,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C19,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O19" s="51">
@@ -7259,7 +7259,7 @@
         <v>252</v>
       </c>
       <c r="Q19" s="56">
-        <f>_xll.XLLInterpolate(P19,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P19,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R19" s="56">
@@ -7267,19 +7267,19 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S19" s="38">
-        <f>_xll.XLLBlack(D19,N19,G19,O19,M19*SQRT(O19/365),1)*H19</f>
-        <v>37859.374284119272</v>
+        <f>_xll.xllBlack(D19,N19,G19,O19,M19*SQRT(O19/365),1)*H19</f>
+        <v>37863.190690330943</v>
       </c>
       <c r="T19" s="57">
         <f t="shared" si="26"/>
-        <v>37520.866440894832</v>
+        <v>37524.648723895007</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="58" customFormat="1">
       <c r="A20" s="49"/>
       <c r="B20" s="49">
         <f t="shared" si="27"/>
-        <v>3.9302974588783508</v>
+        <v>3.9306477392963388</v>
       </c>
       <c r="C20" s="50">
         <v>43097</v>
@@ -7309,22 +7309,22 @@
       </c>
       <c r="J20" s="54">
         <f t="shared" si="24"/>
-        <v>39302.974588783509</v>
+        <v>39306.477392963388</v>
       </c>
       <c r="K20" s="55">
-        <f>_xll.XLLBlackDelta(D20,N20,G20,O20,M20*SQRT(O20/365),1)</f>
-        <v>-0.36545266088160122</v>
+        <f>_xll.xllBlackDelta(D20,N20,G20,O20,M20*SQRT(O20/365),1)</f>
+        <v>-0.36545488048703523</v>
       </c>
       <c r="L20" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D20,N20,G20,O20,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28811944425194508</v>
+        <f>_xll.xllBlackVolOffSurface(D20,N20,G20,O20,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28813992233363023</v>
       </c>
       <c r="M20" s="35">
         <f>L20+0.01</f>
-        <v>0.29811944425194509</v>
+        <v>0.29813992233363024</v>
       </c>
       <c r="N20" s="36">
-        <f>_xll.XLLInterpolate(C20,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C20,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O20" s="51">
@@ -7336,7 +7336,7 @@
         <v>281</v>
       </c>
       <c r="Q20" s="56">
-        <f>_xll.XLLInterpolate(P20,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P20,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R20" s="56">
@@ -7344,18 +7344,18 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S20" s="38">
-        <f>_xll.XLLBlack(D20,N20,G20,O20,M20*SQRT(O20/365),1)*H20</f>
-        <v>39705.695744953184</v>
+        <f>_xll.xllBlack(D20,N20,G20,O20,M20*SQRT(O20/365),1)*H20</f>
+        <v>39709.234440903703</v>
       </c>
       <c r="T20" s="57">
         <f t="shared" si="26"/>
-        <v>39302.974588783509</v>
+        <v>39306.477392963388</v>
       </c>
     </row>
     <row r="21" spans="1:20">
       <c r="B21" s="48">
         <f t="shared" si="27"/>
-        <v>4.354497878370168</v>
+        <v>4.3548734377815155</v>
       </c>
       <c r="C21" s="30">
         <v>43131</v>
@@ -7385,22 +7385,22 @@
       </c>
       <c r="J21" s="20">
         <f t="shared" si="24"/>
-        <v>43544.978783701677</v>
+        <v>43548.734377815155</v>
       </c>
       <c r="K21" s="34">
-        <f>_xll.XLLBlackDelta(D21,N21,G21,O21,M21*SQRT(O21/365),1)</f>
-        <v>-0.36959835257792295</v>
+        <f>_xll.xllBlackDelta(D21,N21,G21,O21,M21*SQRT(O21/365),1)</f>
+        <v>-0.36959975330397976</v>
       </c>
       <c r="L21" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D21,N21,G21,O21,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28334053899632983</v>
+        <f>_xll.xllBlackVolOffSurface(D21,N21,G21,O21,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28336120771860407</v>
       </c>
       <c r="M21" s="35">
         <f>L21+0.02</f>
-        <v>0.30334053899632984</v>
+        <v>0.30336120771860409</v>
       </c>
       <c r="N21" s="36">
-        <f>_xll.XLLInterpolate(C21,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C21,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O21" s="31">
@@ -7412,7 +7412,7 @@
         <v>314</v>
       </c>
       <c r="Q21" s="37">
-        <f>_xll.XLLInterpolate(P21,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P21,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R21" s="37">
@@ -7420,22 +7420,22 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S21" s="38">
-        <f>_xll.XLLBlack(D21,N21,G21,O21,M21*SQRT(O21/365),1)*H21</f>
-        <v>44053.346046176361</v>
+        <f>_xll.xllBlack(D21,N21,G21,O21,M21*SQRT(O21/365),1)*H21</f>
+        <v>44057.145485094719</v>
       </c>
       <c r="T21" s="39">
         <f t="shared" si="26"/>
-        <v>43544.978783701677</v>
+        <v>43548.734377815155</v>
       </c>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="48">
         <f>AVERAGE(B21:B23)</f>
-        <v>4.5405682549659385</v>
+        <v>4.5407002314376212</v>
       </c>
       <c r="B22" s="48">
         <f t="shared" si="27"/>
-        <v>4.5432774008327881</v>
+        <v>4.543289654525938</v>
       </c>
       <c r="C22" s="30">
         <v>43159</v>
@@ -7465,22 +7465,22 @@
       </c>
       <c r="J22" s="20">
         <f t="shared" si="24"/>
-        <v>45432.774008327884</v>
+        <v>45432.896545259384</v>
       </c>
       <c r="K22" s="34">
-        <f>_xll.XLLBlackDelta(D22,N22,G22,O22,M22*SQRT(O22/365),1)</f>
-        <v>-0.3711969177416935</v>
+        <f>_xll.xllBlackDelta(D22,N22,G22,O22,M22*SQRT(O22/365),1)</f>
+        <v>-0.37119693825929057</v>
       </c>
       <c r="L22" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D22,N22,G22,O22,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27991370458014869</v>
+        <f>_xll.xllBlackVolOffSurface(D22,N22,G22,O22,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27991423340969296</v>
       </c>
       <c r="M22" s="35">
         <f>L22+0.02</f>
-        <v>0.29991370458014871</v>
+        <v>0.29991423340969298</v>
       </c>
       <c r="N22" s="36">
-        <f>_xll.XLLInterpolate(C22,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C22,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O22" s="31">
@@ -7492,7 +7492,7 @@
         <v>342</v>
       </c>
       <c r="Q22" s="37">
-        <f>_xll.XLLInterpolate(P22,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P22,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R22" s="37">
@@ -7500,18 +7500,18 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S22" s="38">
-        <f>_xll.XLLBlack(D22,N22,G22,O22,M22*SQRT(O22/365),1)*H22</f>
-        <v>46019.929123514987</v>
+        <f>_xll.xllBlack(D22,N22,G22,O22,M22*SQRT(O22/365),1)*H22</f>
+        <v>46020.053244065086</v>
       </c>
       <c r="T22" s="39">
         <f t="shared" si="26"/>
-        <v>45432.774008327884</v>
+        <v>45432.896545259384</v>
       </c>
     </row>
     <row r="23" spans="1:20">
       <c r="B23" s="48">
         <f t="shared" si="27"/>
-        <v>4.7239294856948586</v>
+        <v>4.7239376020054094</v>
       </c>
       <c r="C23" s="30">
         <v>43188</v>
@@ -7541,22 +7541,22 @@
       </c>
       <c r="J23" s="20">
         <f t="shared" si="24"/>
-        <v>47239.294856948582</v>
+        <v>47239.376020054093</v>
       </c>
       <c r="K23" s="34">
-        <f>_xll.XLLBlackDelta(D23,N23,G23,O23,M23*SQRT(O23/365),1)</f>
-        <v>-0.37281579188009861</v>
+        <f>_xll.xllBlackDelta(D23,N23,G23,O23,M23*SQRT(O23/365),1)</f>
+        <v>-0.37281579543426202</v>
       </c>
       <c r="L23" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D23,N23,G23,O23,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27630227775034483</v>
+        <f>_xll.xllBlackVolOffSurface(D23,N23,G23,O23,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27630259244482691</v>
       </c>
       <c r="M23" s="35">
         <f>L23+0.02</f>
-        <v>0.29630227775034484</v>
+        <v>0.29630259244482693</v>
       </c>
       <c r="N23" s="36">
-        <f>_xll.XLLInterpolate(C23,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C23,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O23" s="31">
@@ -7568,7 +7568,7 @@
         <v>372</v>
       </c>
       <c r="Q23" s="37">
-        <f>_xll.XLLInterpolate(P23,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P23,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R23" s="37">
@@ -7576,19 +7576,19 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S23" s="38">
-        <f>_xll.XLLBlack(D23,N23,G23,O23,M23*SQRT(O23/365),1)*H23</f>
-        <v>47914.729006059497</v>
+        <f>_xll.xllBlack(D23,N23,G23,O23,M23*SQRT(O23/365),1)*H23</f>
+        <v>47914.811329646625</v>
       </c>
       <c r="T23" s="39">
         <f t="shared" si="26"/>
-        <v>47239.294856948582</v>
+        <v>47239.376020054093</v>
       </c>
     </row>
     <row r="24" spans="1:20" s="58" customFormat="1">
       <c r="A24" s="49"/>
       <c r="B24" s="49">
         <f t="shared" si="27"/>
-        <v>5.0609798214240582</v>
+        <v>5.0609824972630815</v>
       </c>
       <c r="C24" s="50">
         <v>43220</v>
@@ -7618,22 +7618,22 @@
       </c>
       <c r="J24" s="54">
         <f t="shared" si="24"/>
-        <v>50609.798214240582</v>
+        <v>50609.824972630813</v>
       </c>
       <c r="K24" s="55">
-        <f>_xll.XLLBlackDelta(D24,N24,G24,O24,M24*SQRT(O24/365),1)</f>
-        <v>-0.37598159117032548</v>
+        <f>_xll.xllBlackDelta(D24,N24,G24,O24,M24*SQRT(O24/365),1)</f>
+        <v>-0.37598158235809376</v>
       </c>
       <c r="L24" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D24,N24,G24,O24,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27372320362648755</v>
+        <f>_xll.xllBlackVolOffSurface(D24,N24,G24,O24,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27372331879253742</v>
       </c>
       <c r="M24" s="35">
         <f>L24+0.025</f>
-        <v>0.29872320362648758</v>
+        <v>0.29872331879253744</v>
       </c>
       <c r="N24" s="36">
-        <f>_xll.XLLInterpolate(C24,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C24,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O24" s="51">
@@ -7645,7 +7645,7 @@
         <v>403</v>
       </c>
       <c r="Q24" s="56">
-        <f>_xll.XLLInterpolate(P24,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P24,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R24" s="56">
@@ -7653,22 +7653,22 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S24" s="38">
-        <f>_xll.XLLBlack(D24,N24,G24,O24,M24*SQRT(O24/365),1)*H24</f>
-        <v>51406.351271873376</v>
+        <f>_xll.xllBlack(D24,N24,G24,O24,M24*SQRT(O24/365),1)*H24</f>
+        <v>51406.378451416793</v>
       </c>
       <c r="T24" s="57">
         <f t="shared" si="26"/>
-        <v>50609.798214240582</v>
+        <v>50609.824972630813</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="58" customFormat="1">
       <c r="A25" s="49">
         <f>AVERAGE(B24:B26)</f>
-        <v>5.2468238731990597</v>
+        <v>5.2468889075195522</v>
       </c>
       <c r="B25" s="49">
         <f t="shared" si="27"/>
-        <v>5.2510890569370465</v>
+        <v>5.2512817255302053</v>
       </c>
       <c r="C25" s="50">
         <v>43251</v>
@@ -7698,22 +7698,22 @@
       </c>
       <c r="J25" s="54">
         <f t="shared" si="24"/>
-        <v>52510.890569370466</v>
+        <v>52512.817255302056</v>
       </c>
       <c r="K25" s="55">
-        <f>_xll.XLLBlackDelta(D25,N25,G25,O25,M25*SQRT(O25/365),1)</f>
-        <v>-0.37711353958668115</v>
+        <f>_xll.xllBlackDelta(D25,N25,G25,O25,M25*SQRT(O25/365),1)</f>
+        <v>-0.37711344566546012</v>
       </c>
       <c r="L25" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D25,N25,G25,O25,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27111321981746561</v>
+        <f>_xll.xllBlackVolOffSurface(D25,N25,G25,O25,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27112228252390913</v>
       </c>
       <c r="M25" s="35">
         <f>L25+0.025</f>
-        <v>0.29611321981746563</v>
+        <v>0.29612228252390915</v>
       </c>
       <c r="N25" s="36">
-        <f>_xll.XLLInterpolate(C25,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C25,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O25" s="51">
@@ -7725,7 +7725,7 @@
         <v>434</v>
       </c>
       <c r="Q25" s="56">
-        <f>_xll.XLLInterpolate(P25,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P25,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R25" s="56">
@@ -7733,19 +7733,19 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S25" s="38">
-        <f>_xll.XLLBlack(D25,N25,G25,O25,M25*SQRT(O25/365),1)*H25</f>
-        <v>53415.080158071825</v>
+        <f>_xll.xllBlack(D25,N25,G25,O25,M25*SQRT(O25/365),1)*H25</f>
+        <v>53417.04001977593</v>
       </c>
       <c r="T25" s="57">
         <f t="shared" si="26"/>
-        <v>52510.890569370466</v>
+        <v>52512.817255302056</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="58" customFormat="1">
       <c r="A26" s="49"/>
       <c r="B26" s="49">
         <f t="shared" si="27"/>
-        <v>5.4284027412360736</v>
+        <v>5.4284024997653697</v>
       </c>
       <c r="C26" s="50">
         <v>43280</v>
@@ -7775,22 +7775,22 @@
       </c>
       <c r="J26" s="54">
         <f t="shared" si="24"/>
-        <v>54284.027412360738</v>
+        <v>54284.024997653694</v>
       </c>
       <c r="K26" s="55">
-        <f>_xll.XLLBlackDelta(D26,N26,G26,O26,M26*SQRT(O26/365),1)</f>
-        <v>-0.3783270676071675</v>
+        <f>_xll.xllBlackDelta(D26,N26,G26,O26,M26*SQRT(O26/365),1)</f>
+        <v>-0.37832705670325517</v>
       </c>
       <c r="L26" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D26,N26,G26,O26,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.26896240418409767</v>
+        <f>_xll.xllBlackVolOffSurface(D26,N26,G26,O26,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.26896241362104312</v>
       </c>
       <c r="M26" s="35">
         <f>L26+0.025</f>
-        <v>0.29396240418409769</v>
+        <v>0.29396241362104314</v>
       </c>
       <c r="N26" s="36">
-        <f>_xll.XLLInterpolate(C26,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C26,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O26" s="51">
@@ -7802,7 +7802,7 @@
         <v>463</v>
       </c>
       <c r="Q26" s="56">
-        <f>_xll.XLLInterpolate(P26,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P26,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R26" s="56">
@@ -7810,18 +7810,18 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S26" s="38">
-        <f>_xll.XLLBlack(D26,N26,G26,O26,M26*SQRT(O26/365),1)*H26</f>
-        <v>55295.841121198988</v>
+        <f>_xll.xllBlack(D26,N26,G26,O26,M26*SQRT(O26/365),1)*H26</f>
+        <v>55295.838661483605</v>
       </c>
       <c r="T26" s="57">
         <f t="shared" si="26"/>
-        <v>54284.027412360738</v>
+        <v>54284.024997653694</v>
       </c>
     </row>
     <row r="28" spans="1:20">
       <c r="B28" s="48">
         <f>J28/H28</f>
-        <v>3.2266225319849919</v>
+        <v>3.2265671295121612</v>
       </c>
       <c r="C28" s="30">
         <v>42947</v>
@@ -7847,22 +7847,22 @@
       </c>
       <c r="J28" s="20">
         <f t="shared" ref="J28:J39" si="32">T28</f>
-        <v>32266.22531984992</v>
+        <v>32265.67129512161</v>
       </c>
       <c r="K28" s="34">
-        <f>_xll.XLLBlackDelta(D28,N28,G28,O28,M28*SQRT(O28/365),1)</f>
-        <v>-0.42936088178478182</v>
+        <f>_xll.xllBlackDelta(D28,N28,G28,O28,M28*SQRT(O28/365),1)</f>
+        <v>-0.42936085127013446</v>
       </c>
       <c r="L28" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D28,N28,G28,O28,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.30028598775958942</v>
+        <f>_xll.xllBlackVolOffSurface(D28,N28,G28,O28,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.30028135827806668</v>
       </c>
       <c r="M28" s="35">
         <f>L28</f>
-        <v>0.30028598775958942</v>
+        <v>0.30028135827806668</v>
       </c>
       <c r="N28" s="36">
-        <f>_xll.XLLInterpolate(C28,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C28,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O28" s="31">
@@ -7874,7 +7874,7 @@
         <v>130</v>
       </c>
       <c r="Q28" s="37">
-        <f>_xll.XLLInterpolate(P28,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P28,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R28" s="37">
@@ -7882,22 +7882,22 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S28" s="38">
-        <f>_xll.XLLBlack(D28,N28,G28,O28,M28*SQRT(O28/365),1)*H28</f>
-        <v>32404.408815818933</v>
+        <f>_xll.xllBlack(D28,N28,G28,O28,M28*SQRT(O28/365),1)*H28</f>
+        <v>32403.852418421586</v>
       </c>
       <c r="T28" s="39">
         <f t="shared" ref="T28:T39" si="34">S28*R28</f>
-        <v>32266.22531984992</v>
+        <v>32265.67129512161</v>
       </c>
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="48">
         <f>AVERAGE(B28:B30)</f>
-        <v>3.5876787851397238</v>
+        <v>3.5878491044892953</v>
       </c>
       <c r="B29" s="48">
         <f t="shared" ref="B29:B39" si="35">J29/H29</f>
-        <v>3.613207394425979</v>
+        <v>3.613773704002802</v>
       </c>
       <c r="C29" s="30">
         <v>42978</v>
@@ -7927,22 +7927,22 @@
       </c>
       <c r="J29" s="20">
         <f t="shared" si="32"/>
-        <v>36132.073944259791</v>
+        <v>36137.73704002802</v>
       </c>
       <c r="K29" s="34">
-        <f>_xll.XLLBlackDelta(D29,N29,G29,O29,M29*SQRT(O29/365),1)</f>
-        <v>-0.42681034384066674</v>
+        <f>_xll.xllBlackDelta(D29,N29,G29,O29,M29*SQRT(O29/365),1)</f>
+        <v>-0.42680978137342407</v>
       </c>
       <c r="L29" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D29,N29,G29,O29,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29939046993952045</v>
+        <f>_xll.xllBlackVolOffSurface(D29,N29,G29,O29,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.29943271260105442</v>
       </c>
       <c r="M29" s="35">
         <f t="shared" ref="M29:M30" si="38">L29</f>
-        <v>0.29939046993952045</v>
+        <v>0.29943271260105442</v>
       </c>
       <c r="N29" s="36">
-        <f>_xll.XLLInterpolate(C29,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C29,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O29" s="31">
@@ -7954,7 +7954,7 @@
         <v>161</v>
       </c>
       <c r="Q29" s="37">
-        <f>_xll.XLLInterpolate(P29,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P29,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R29" s="37">
@@ -7962,18 +7962,18 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S29" s="38">
-        <f>_xll.XLLBlack(D29,N29,G29,O29,M29*SQRT(O29/365),1)*H29</f>
-        <v>36328.040332313838</v>
+        <f>_xll.xllBlack(D29,N29,G29,O29,M29*SQRT(O29/365),1)*H29</f>
+        <v>36333.734142522226</v>
       </c>
       <c r="T29" s="39">
         <f t="shared" si="34"/>
-        <v>36132.073944259791</v>
+        <v>36137.73704002802</v>
       </c>
     </row>
     <row r="30" spans="1:20">
       <c r="B30" s="48">
         <f t="shared" si="35"/>
-        <v>3.9232064290082009</v>
+        <v>3.9232064799529232</v>
       </c>
       <c r="C30" s="30">
         <v>43007</v>
@@ -8003,22 +8003,22 @@
       </c>
       <c r="J30" s="20">
         <f t="shared" si="32"/>
-        <v>39232.064290082009</v>
+        <v>39232.064799529231</v>
       </c>
       <c r="K30" s="34">
-        <f>_xll.XLLBlackDelta(D30,N30,G30,O30,M30*SQRT(O30/365),1)</f>
-        <v>-0.42558531000465427</v>
+        <f>_xll.xllBlackDelta(D30,N30,G30,O30,M30*SQRT(O30/365),1)</f>
+        <v>-0.4255852974904103</v>
       </c>
       <c r="L30" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D30,N30,G30,O30,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29674375887644339</v>
+        <f>_xll.xllBlackVolOffSurface(D30,N30,G30,O30,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.29674381144091944</v>
       </c>
       <c r="M30" s="35">
         <f t="shared" si="38"/>
-        <v>0.29674375887644339</v>
+        <v>0.29674381144091944</v>
       </c>
       <c r="N30" s="36">
-        <f>_xll.XLLInterpolate(C30,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.xllInterpolate(C30,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O30" s="31">
@@ -8030,7 +8030,7 @@
         <v>190</v>
       </c>
       <c r="Q30" s="37">
-        <f>_xll.XLLInterpolate(P30,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P30,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R30" s="37">
@@ -8038,19 +8038,19 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S30" s="38">
-        <f>_xll.XLLBlack(D30,N30,G30,O30,M30*SQRT(O30/365),1)*H30</f>
-        <v>39488.340822248421</v>
+        <f>_xll.xllBlack(D30,N30,G30,O30,M30*SQRT(O30/365),1)*H30</f>
+        <v>39488.341335023521</v>
       </c>
       <c r="T30" s="39">
         <f t="shared" si="34"/>
-        <v>39232.064290082009</v>
+        <v>39232.064799529231</v>
       </c>
     </row>
     <row r="31" spans="1:20" s="58" customFormat="1">
       <c r="A31" s="49"/>
       <c r="B31" s="49">
         <f t="shared" si="35"/>
-        <v>4.4180280233736067</v>
+        <v>4.4184538435842189</v>
       </c>
       <c r="C31" s="50">
         <v>43039</v>
@@ -8080,22 +8080,22 @@
       </c>
       <c r="J31" s="54">
         <f t="shared" si="32"/>
-        <v>44180.28023373607</v>
+        <v>44184.538435842187</v>
       </c>
       <c r="K31" s="55">
-        <f>_xll.XLLBlackDelta(D31,N31,G31,O31,M31*SQRT(O31/365),1)</f>
-        <v>-0.42550634330150594</v>
+        <f>_xll.xllBlackDelta(D31,N31,G31,O31,M31*SQRT(O31/365),1)</f>
+        <v>-0.42550473632764729</v>
       </c>
       <c r="L31" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D31,N31,G31,O31,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.29435273084736541</v>
+        <f>_xll.xllBlackVolOffSurface(D31,N31,G31,O31,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.29437980749351916</v>
       </c>
       <c r="M31" s="35">
         <f>L31+0.01</f>
-        <v>0.30435273084736542</v>
+        <v>0.30437980749351917</v>
       </c>
       <c r="N31" s="36">
-        <f>_xll.XLLInterpolate(C31,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C31,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O31" s="51">
@@ -8107,7 +8107,7 @@
         <v>222</v>
       </c>
       <c r="Q31" s="56">
-        <f>_xll.XLLInterpolate(P31,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P31,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R31" s="56">
@@ -8115,22 +8115,22 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S31" s="38">
-        <f>_xll.XLLBlack(D31,N31,G31,O31,M31*SQRT(O31/365),1)*H31</f>
-        <v>44524.669503028243</v>
+        <f>_xll.xllBlack(D31,N31,G31,O31,M31*SQRT(O31/365),1)*H31</f>
+        <v>44528.960898203848</v>
       </c>
       <c r="T31" s="57">
         <f t="shared" si="34"/>
-        <v>44180.28023373607</v>
+        <v>44184.538435842187</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="58" customFormat="1">
       <c r="A32" s="49">
         <f>AVERAGE(B31:B33)</f>
-        <v>4.6217807444380794</v>
+        <v>4.6221408972751297</v>
       </c>
       <c r="B32" s="49">
         <f t="shared" si="35"/>
-        <v>4.6281356049490139</v>
+        <v>4.6284700241535193</v>
       </c>
       <c r="C32" s="50">
         <v>43069</v>
@@ -8160,22 +8160,22 @@
       </c>
       <c r="J32" s="54">
         <f t="shared" si="32"/>
-        <v>46281.356049490139</v>
+        <v>46284.700241535189</v>
       </c>
       <c r="K32" s="55">
-        <f>_xll.XLLBlackDelta(D32,N32,G32,O32,M32*SQRT(O32/365),1)</f>
-        <v>-0.42464693689314092</v>
+        <f>_xll.xllBlackDelta(D32,N32,G32,O32,M32*SQRT(O32/365),1)</f>
+        <v>-0.42464550509498566</v>
       </c>
       <c r="L32" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D32,N32,G32,O32,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.28791911328514069</v>
+        <f>_xll.xllBlackVolOffSurface(D32,N32,G32,O32,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28793908707932159</v>
       </c>
       <c r="M32" s="35">
         <f>L32+0.01</f>
-        <v>0.2979191132851407</v>
+        <v>0.2979390870793216</v>
       </c>
       <c r="N32" s="36">
-        <f>_xll.XLLInterpolate(C32,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C32,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O32" s="51">
@@ -8187,7 +8187,7 @@
         <v>252</v>
       </c>
       <c r="Q32" s="56">
-        <f>_xll.XLLInterpolate(P32,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P32,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R32" s="56">
@@ -8195,19 +8195,19 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S32" s="38">
-        <f>_xll.XLLBlack(D32,N32,G32,O32,M32*SQRT(O32/365),1)*H32</f>
-        <v>46698.899765931084</v>
+        <f>_xll.xllBlack(D32,N32,G32,O32,M32*SQRT(O32/365),1)*H32</f>
+        <v>46702.274128794234</v>
       </c>
       <c r="T32" s="57">
         <f t="shared" si="34"/>
-        <v>46281.356049490139</v>
+        <v>46284.700241535189</v>
       </c>
     </row>
     <row r="33" spans="1:20" s="58" customFormat="1">
       <c r="A33" s="49"/>
       <c r="B33" s="49">
         <f t="shared" si="35"/>
-        <v>4.8191786049916177</v>
+        <v>4.8194988240876482</v>
       </c>
       <c r="C33" s="50">
         <v>43097</v>
@@ -8237,22 +8237,22 @@
       </c>
       <c r="J33" s="54">
         <f t="shared" si="32"/>
-        <v>48191.786049916176</v>
+        <v>48194.988240876482</v>
       </c>
       <c r="K33" s="55">
-        <f>_xll.XLLBlackDelta(D33,N33,G33,O33,M33*SQRT(O33/365),1)</f>
-        <v>-0.42439902340899816</v>
+        <f>_xll.xllBlackDelta(D33,N33,G33,O33,M33*SQRT(O33/365),1)</f>
+        <v>-0.42439749124093862</v>
       </c>
       <c r="L33" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D33,N33,G33,O33,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.2828462473803407</v>
+        <f>_xll.xllBlackVolOffSurface(D33,N33,G33,O33,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.28286439866994223</v>
       </c>
       <c r="M33" s="35">
         <f>L33+0.01</f>
-        <v>0.29284624738034071</v>
+        <v>0.29286439866994224</v>
       </c>
       <c r="N33" s="36">
-        <f>_xll.XLLInterpolate(C33,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.xllInterpolate(C33,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O33" s="51">
@@ -8264,7 +8264,7 @@
         <v>281</v>
       </c>
       <c r="Q33" s="56">
-        <f>_xll.XLLInterpolate(P33,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P33,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R33" s="56">
@@ -8272,18 +8272,18 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S33" s="38">
-        <f>_xll.XLLBlack(D33,N33,G33,O33,M33*SQRT(O33/365),1)*H33</f>
-        <v>48685.587142555174</v>
+        <f>_xll.xllBlack(D33,N33,G33,O33,M33*SQRT(O33/365),1)*H33</f>
+        <v>48688.822145028076</v>
       </c>
       <c r="T33" s="57">
         <f t="shared" si="34"/>
-        <v>48191.786049916176</v>
+        <v>48194.988240876482</v>
       </c>
     </row>
     <row r="34" spans="1:20">
       <c r="B34" s="48">
         <f t="shared" si="35"/>
-        <v>5.265808020362222</v>
+        <v>5.2661669155425983</v>
       </c>
       <c r="C34" s="30">
         <v>43131</v>
@@ -8313,22 +8313,22 @@
       </c>
       <c r="J34" s="20">
         <f t="shared" si="32"/>
-        <v>52658.080203622216</v>
+        <v>52661.669155425981</v>
       </c>
       <c r="K34" s="34">
-        <f>_xll.XLLBlackDelta(D34,N34,G34,O34,M34*SQRT(O34/365),1)</f>
-        <v>-0.42442568027853711</v>
+        <f>_xll.xllBlackDelta(D34,N34,G34,O34,M34*SQRT(O34/365),1)</f>
+        <v>-0.42442357038188716</v>
       </c>
       <c r="L34" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D34,N34,G34,O34,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27854058477499272</v>
+        <f>_xll.xllBlackVolOffSurface(D34,N34,G34,O34,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27855979919652529</v>
       </c>
       <c r="M34" s="35">
         <f>L34+0.02</f>
-        <v>0.29854058477499273</v>
+        <v>0.29855979919652531</v>
       </c>
       <c r="N34" s="36">
-        <f>_xll.XLLInterpolate(C34,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C34,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O34" s="31">
@@ -8340,7 +8340,7 @@
         <v>314</v>
       </c>
       <c r="Q34" s="37">
-        <f>_xll.XLLInterpolate(P34,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P34,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R34" s="37">
@@ -8348,22 +8348,22 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S34" s="38">
-        <f>_xll.XLLBlack(D34,N34,G34,O34,M34*SQRT(O34/365),1)*H34</f>
-        <v>53272.83866322002</v>
+        <f>_xll.xllBlack(D34,N34,G34,O34,M34*SQRT(O34/365),1)*H34</f>
+        <v>53276.469514357639</v>
       </c>
       <c r="T34" s="39">
         <f t="shared" si="34"/>
-        <v>52658.080203622216</v>
+        <v>52661.669155425981</v>
       </c>
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="48">
         <f>AVERAGE(B34:B36)</f>
-        <v>5.4621544475168031</v>
+        <v>5.4622789587750828</v>
       </c>
       <c r="B35" s="48">
         <f t="shared" si="35"/>
-        <v>5.4652358260511233</v>
+        <v>5.4652425754458429</v>
       </c>
       <c r="C35" s="30">
         <v>43159</v>
@@ -8393,22 +8393,22 @@
       </c>
       <c r="J35" s="20">
         <f t="shared" si="32"/>
-        <v>54652.358260511231</v>
+        <v>54652.425754458432</v>
       </c>
       <c r="K35" s="34">
-        <f>_xll.XLLBlackDelta(D35,N35,G35,O35,M35*SQRT(O35/365),1)</f>
-        <v>-0.42434787099903881</v>
+        <f>_xll.xllBlackDelta(D35,N35,G35,O35,M35*SQRT(O35/365),1)</f>
+        <v>-0.42434781074794536</v>
       </c>
       <c r="L35" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D35,N35,G35,O35,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27547029485396302</v>
+        <f>_xll.xllBlackVolOffSurface(D35,N35,G35,O35,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.27547069125621454</v>
       </c>
       <c r="M35" s="35">
         <f>L35+0.02</f>
-        <v>0.29547029485396303</v>
+        <v>0.29547069125621456</v>
       </c>
       <c r="N35" s="36">
-        <f>_xll.XLLInterpolate(C35,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C35,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O35" s="31">
@@ -8420,7 +8420,7 @@
         <v>342</v>
       </c>
       <c r="Q35" s="37">
-        <f>_xll.XLLInterpolate(P35,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P35,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R35" s="37">
@@ -8428,18 +8428,18 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S35" s="38">
-        <f>_xll.XLLBlack(D35,N35,G35,O35,M35*SQRT(O35/365),1)*H35</f>
-        <v>55358.663618485087</v>
+        <f>_xll.xllBlack(D35,N35,G35,O35,M35*SQRT(O35/365),1)*H35</f>
+        <v>55358.731984697231</v>
       </c>
       <c r="T35" s="39">
         <f t="shared" si="34"/>
-        <v>54652.358260511231</v>
+        <v>54652.425754458432</v>
       </c>
     </row>
     <row r="36" spans="1:20">
       <c r="B36" s="48">
         <f t="shared" si="35"/>
-        <v>5.6554194961370641</v>
+        <v>5.6554273853368064</v>
       </c>
       <c r="C36" s="30">
         <v>43188</v>
@@ -8469,22 +8469,22 @@
       </c>
       <c r="J36" s="20">
         <f t="shared" si="32"/>
-        <v>56554.194961370638</v>
+        <v>56554.27385336806</v>
       </c>
       <c r="K36" s="34">
-        <f>_xll.XLLBlackDelta(D36,N36,G36,O36,M36*SQRT(O36/365),1)</f>
-        <v>-0.42449574494705611</v>
+        <f>_xll.xllBlackDelta(D36,N36,G36,O36,M36*SQRT(O36/365),1)</f>
+        <v>-0.42449567535457533</v>
       </c>
       <c r="L36" s="34">
-        <f>_xll.XLLBlackVolOffSurface(D36,N36,G36,O36,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.27214638861479001</v>
+        <f>_xll.xllBlackVolOffSurface(D36,N36,G36,O36,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.2721468149249171</v>
       </c>
       <c r="M36" s="35">
         <f>L36+0.02</f>
-        <v>0.29214638861479003</v>
+        <v>0.29214681492491712</v>
       </c>
       <c r="N36" s="36">
-        <f>_xll.XLLInterpolate(C36,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.xllInterpolate(C36,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O36" s="31">
@@ -8496,7 +8496,7 @@
         <v>372</v>
       </c>
       <c r="Q36" s="37">
-        <f>_xll.XLLInterpolate(P36,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P36,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R36" s="37">
@@ -8504,19 +8504,19 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S36" s="38">
-        <f>_xll.XLLBlack(D36,N36,G36,O36,M36*SQRT(O36/365),1)*H36</f>
-        <v>57362.814875534481</v>
+        <f>_xll.xllBlack(D36,N36,G36,O36,M36*SQRT(O36/365),1)*H36</f>
+        <v>57362.894895540892</v>
       </c>
       <c r="T36" s="39">
         <f t="shared" si="34"/>
-        <v>56554.194961370638</v>
+        <v>56554.27385336806</v>
       </c>
     </row>
     <row r="37" spans="1:20" s="58" customFormat="1">
       <c r="A37" s="49"/>
       <c r="B37" s="49">
         <f t="shared" si="35"/>
-        <v>6.0086167659952308</v>
+        <v>6.0086280429461576</v>
       </c>
       <c r="C37" s="50">
         <v>43220</v>
@@ -8546,22 +8546,22 @@
       </c>
       <c r="J37" s="54">
         <f t="shared" si="32"/>
-        <v>60086.167659952305</v>
+        <v>60086.280429461578</v>
       </c>
       <c r="K37" s="55">
-        <f>_xll.XLLBlackDelta(D37,N37,G37,O37,M37*SQRT(O37/365),1)</f>
-        <v>-0.42527476418048371</v>
+        <f>_xll.xllBlackDelta(D37,N37,G37,O37,M37*SQRT(O37/365),1)</f>
+        <v>-0.42527466628415733</v>
       </c>
       <c r="L37" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D37,N37,G37,O37,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.26980323013515839</v>
+        <f>_xll.xllBlackVolOffSurface(D37,N37,G37,O37,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.26980378002809019</v>
       </c>
       <c r="M37" s="35">
         <f>L37+0.025</f>
-        <v>0.29480323013515841</v>
+        <v>0.29480378002809021</v>
       </c>
       <c r="N37" s="36">
-        <f>_xll.XLLInterpolate(C37,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C37,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O37" s="51">
@@ -8573,7 +8573,7 @@
         <v>403</v>
       </c>
       <c r="Q37" s="56">
-        <f>_xll.XLLInterpolate(P37,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P37,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R37" s="56">
@@ -8581,22 +8581,22 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S37" s="38">
-        <f>_xll.XLLBlack(D37,N37,G37,O37,M37*SQRT(O37/365),1)*H37</f>
-        <v>61031.8703155599</v>
+        <f>_xll.xllBlack(D37,N37,G37,O37,M37*SQRT(O37/365),1)*H37</f>
+        <v>61031.984859960605</v>
       </c>
       <c r="T37" s="57">
         <f t="shared" si="34"/>
-        <v>60086.167659952305</v>
+        <v>60086.280429461578</v>
       </c>
     </row>
     <row r="38" spans="1:20" s="58" customFormat="1">
       <c r="A38" s="49">
         <f>AVERAGE(B37:B39)</f>
-        <v>6.2043146483904126</v>
+        <v>6.2043907864916967</v>
       </c>
       <c r="B38" s="49">
         <f t="shared" si="35"/>
-        <v>6.2096477539128259</v>
+        <v>6.2098511986835092</v>
       </c>
       <c r="C38" s="50">
         <v>43251</v>
@@ -8626,22 +8626,22 @@
       </c>
       <c r="J38" s="54">
         <f t="shared" si="32"/>
-        <v>62096.47753912826</v>
+        <v>62098.511986835096</v>
       </c>
       <c r="K38" s="55">
-        <f>_xll.XLLBlackDelta(D38,N38,G38,O38,M38*SQRT(O38/365),1)</f>
-        <v>-0.42502826947059336</v>
+        <f>_xll.xllBlackDelta(D38,N38,G38,O38,M38*SQRT(O38/365),1)</f>
+        <v>-0.42502667104308745</v>
       </c>
       <c r="L38" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D38,N38,G38,O38,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.26752805115759809</v>
+        <f>_xll.xllBlackVolOffSurface(D38,N38,G38,O38,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.26753735396207162</v>
       </c>
       <c r="M38" s="35">
         <f>L38+0.025</f>
-        <v>0.29252805115759811</v>
+        <v>0.29253735396207164</v>
       </c>
       <c r="N38" s="36">
-        <f>_xll.XLLInterpolate(C38,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C38,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O38" s="51">
@@ -8653,7 +8653,7 @@
         <v>434</v>
       </c>
       <c r="Q38" s="56">
-        <f>_xll.XLLInterpolate(P38,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P38,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R38" s="56">
@@ -8661,19 +8661,19 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S38" s="38">
-        <f>_xll.XLLBlack(D38,N38,G38,O38,M38*SQRT(O38/365),1)*H38</f>
-        <v>63165.722182993777</v>
+        <f>_xll.xllBlack(D38,N38,G38,O38,M38*SQRT(O38/365),1)*H38</f>
+        <v>63167.791662032505</v>
       </c>
       <c r="T38" s="57">
         <f t="shared" si="34"/>
-        <v>62096.47753912826</v>
+        <v>62098.511986835096</v>
       </c>
     </row>
     <row r="39" spans="1:20" s="58" customFormat="1">
       <c r="A39" s="49"/>
       <c r="B39" s="49">
         <f t="shared" si="35"/>
-        <v>6.3946794252631793</v>
+        <v>6.3946931178454252</v>
       </c>
       <c r="C39" s="50">
         <v>43280</v>
@@ -8703,22 +8703,22 @@
       </c>
       <c r="J39" s="54">
         <f t="shared" si="32"/>
-        <v>63946.794252631793</v>
+        <v>63946.931178454251</v>
       </c>
       <c r="K39" s="55">
-        <f>_xll.XLLBlackDelta(D39,N39,G39,O39,M39*SQRT(O39/365),1)</f>
-        <v>-0.42508206390540892</v>
+        <f>_xll.xllBlackDelta(D39,N39,G39,O39,M39*SQRT(O39/365),1)</f>
+        <v>-0.42508194233890251</v>
       </c>
       <c r="L39" s="55">
-        <f>_xll.XLLBlackVolOffSurface(D39,N39,G39,O39,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
-        <v>0.26554691368424477</v>
+        <f>_xll.xllBlackVolOffSurface(D39,N39,G39,O39,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <v>0.26554751559010453</v>
       </c>
       <c r="M39" s="35">
         <f>L39+0.025</f>
-        <v>0.29054691368424479</v>
+        <v>0.29054751559010455</v>
       </c>
       <c r="N39" s="36">
-        <f>_xll.XLLInterpolate(C39,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.xllInterpolate(C39,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O39" s="51">
@@ -8730,7 +8730,7 @@
         <v>463</v>
       </c>
       <c r="Q39" s="56">
-        <f>_xll.XLLInterpolate(P39,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.xllInterpolate(P39,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R39" s="56">
@@ -8738,12 +8738,29 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S39" s="38">
-        <f>_xll.XLLBlack(D39,N39,G39,O39,M39*SQRT(O39/365),1)*H39</f>
-        <v>65138.714715156995</v>
+        <f>_xll.xllBlack(D39,N39,G39,O39,M39*SQRT(O39/365),1)*H39</f>
+        <v>65138.854193174469</v>
       </c>
       <c r="T39" s="57">
         <f t="shared" si="34"/>
-        <v>63946.794252631793</v>
+        <v>63946.931178454251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="J40" s="20">
+        <f>SUM(J2:J39)</f>
+        <v>1480404.2244890712</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="J41" s="18">
+        <v>1480335.0956798368</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="J42" s="20">
+        <f>J41-J40</f>
+        <v>-69.128809234360233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidy up excel interface
</commit_message>
<xml_diff>
--- a/ExampleSpreadsheet/ICE Brent Options - Fixed Inputs.xlsx
+++ b/ExampleSpreadsheet/ICE Brent Options - Fixed Inputs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="12405" tabRatio="708" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="12405" tabRatio="708"/>
   </bookViews>
   <sheets>
     <sheet name="LCO Vol Surf" sheetId="1" r:id="rId1"/>
@@ -1440,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1451,7 +1451,7 @@
     <col min="19" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1569,7 +1569,7 @@
       </c>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>42830</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>42837</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>42844</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1816,8 +1816,12 @@
       <c r="T6" s="2">
         <v>42857</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="W6">
+        <f>_xll.BlackVolOffSurface("p",100,125,325,S2:S29,B30:R30,B2:R29,0.0001,"bicubic")</f>
+        <v>0.25019944588015197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1879,7 +1883,7 @@
         <v>42885</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:23">
       <c r="A8" s="7" t="s">
         <v>22</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>42915</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:23">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -2003,7 +2007,7 @@
         <v>42947</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:23">
       <c r="A10" s="7" t="s">
         <v>24</v>
       </c>
@@ -2065,7 +2069,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:23">
       <c r="A11" s="7" t="s">
         <v>25</v>
       </c>
@@ -2127,7 +2131,7 @@
         <v>43007</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:23">
       <c r="A12" s="7" t="s">
         <v>26</v>
       </c>
@@ -2189,7 +2193,7 @@
         <v>43038</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:23">
       <c r="A13" s="7" t="s">
         <v>27</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>43068</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:23">
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
@@ -2313,7 +2317,7 @@
         <v>43098</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:23">
       <c r="A15" s="7" t="s">
         <v>29</v>
       </c>
@@ -2375,7 +2379,7 @@
         <v>43129</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:23">
       <c r="A16" s="7" t="s">
         <v>30</v>
       </c>
@@ -3307,12 +3311,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" style="16" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="16" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="40"/>
@@ -4491,9 +4498,9 @@
   </sheetPr>
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="12.75"/>
@@ -4512,7 +4519,7 @@
     <col min="14" max="14" width="8.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="18" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="18" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="20" customWidth="1"/>
+    <col min="17" max="17" width="38.5703125" style="20" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" style="20" customWidth="1"/>
     <col min="19" max="20" width="12.7109375" style="21" customWidth="1"/>
     <col min="21" max="251" width="7.5703125" style="18"/>
@@ -5994,11 +6001,11 @@
         <v>17662.328205052363</v>
       </c>
       <c r="K2" s="34">
-        <f>_xll.xllBlackDelta(D2,N2,G2,O2,M2*SQRT(O2/365),1)</f>
+        <f>_xll.BlackDelta(D2,N2,G2,O2,M2*SQRT(O2/365),1)</f>
         <v>-0.27010976321434743</v>
       </c>
       <c r="L2" s="34">
-        <f>_xll.xllBlackVolOffSurface(D2,N2,G2,O2,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D2,N2,G2,O2,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.31740638936155174</v>
       </c>
       <c r="M2" s="35">
@@ -6006,7 +6013,7 @@
         <v>0.31740638936155174</v>
       </c>
       <c r="N2" s="36">
-        <f>_xll.xllInterpolate(C2,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C2,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O2" s="31">
@@ -6018,7 +6025,7 @@
         <v>130</v>
       </c>
       <c r="Q2" s="37">
-        <f>_xll.xllInterpolate(P2,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P2,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R2" s="37">
@@ -6026,7 +6033,7 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S2" s="38">
-        <f>_xll.xllBlack(D2,N2,G2,O2,M2*SQRT(O2/365),1)*H2</f>
+        <f>_xll.Black(D2,N2,G2,O2,M2*SQRT(O2/365),1)*H2</f>
         <v>17737.968979085661</v>
       </c>
       <c r="T2" s="39">
@@ -6074,11 +6081,11 @@
         <v>21030.879788711616</v>
       </c>
       <c r="K3" s="34">
-        <f>_xll.xllBlackDelta(D3,N3,G3,O3,M3*SQRT(O3/365),1)</f>
+        <f>_xll.BlackDelta(D3,N3,G3,O3,M3*SQRT(O3/365),1)</f>
         <v>-0.28206908288853993</v>
       </c>
       <c r="L3" s="34">
-        <f>_xll.xllBlackVolOffSurface(D3,N3,G3,O3,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D3,N3,G3,O3,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.31477880660800961</v>
       </c>
       <c r="M3" s="35">
@@ -6086,7 +6093,7 @@
         <v>0.31477880660800961</v>
       </c>
       <c r="N3" s="36">
-        <f>_xll.xllInterpolate(C3,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C3,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O3" s="31">
@@ -6098,7 +6105,7 @@
         <v>161</v>
       </c>
       <c r="Q3" s="37">
-        <f>_xll.xllInterpolate(P3,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P3,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R3" s="37">
@@ -6106,7 +6113,7 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S3" s="38">
-        <f>_xll.xllBlack(D3,N3,G3,O3,M3*SQRT(O3/365),1)*H3</f>
+        <f>_xll.Black(D3,N3,G3,O3,M3*SQRT(O3/365),1)*H3</f>
         <v>21144.943142953351</v>
       </c>
       <c r="T3" s="39">
@@ -6150,11 +6157,11 @@
         <v>23737.053994035319</v>
       </c>
       <c r="K4" s="34">
-        <f>_xll.xllBlackDelta(D4,N4,G4,O4,M4*SQRT(O4/365),1)</f>
+        <f>_xll.BlackDelta(D4,N4,G4,O4,M4*SQRT(O4/365),1)</f>
         <v>-0.29026303702914058</v>
       </c>
       <c r="L4" s="34">
-        <f>_xll.xllBlackVolOffSurface(D4,N4,G4,O4,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D4,N4,G4,O4,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.31076843555617095</v>
       </c>
       <c r="M4" s="35">
@@ -6162,7 +6169,7 @@
         <v>0.31076843555617095</v>
       </c>
       <c r="N4" s="36">
-        <f>_xll.xllInterpolate(C4,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C4,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O4" s="31">
@@ -6170,11 +6177,11 @@
         <v>183</v>
       </c>
       <c r="P4" s="31">
-        <f>I4-Rates!$D$1</f>
+        <f>(I4-Rates!$D$1)</f>
         <v>190</v>
       </c>
       <c r="Q4" s="37">
-        <f>_xll.xllInterpolate(P4,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P4,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R4" s="37">
@@ -6182,7 +6189,7 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S4" s="38">
-        <f>_xll.xllBlack(D4,N4,G4,O4,M4*SQRT(O4/365),1)*H4</f>
+        <f>_xll.Black(D4,N4,G4,O4,M4*SQRT(O4/365),1)*H4</f>
         <v>23892.112107634915</v>
       </c>
       <c r="T4" s="39">
@@ -6227,11 +6234,11 @@
         <v>28123.74518459884</v>
       </c>
       <c r="K5" s="55">
-        <f>_xll.xllBlackDelta(D5,N5,G5,O5,M5*SQRT(O5/365),1)</f>
+        <f>_xll.BlackDelta(D5,N5,G5,O5,M5*SQRT(O5/365),1)</f>
         <v>-0.30210950670851022</v>
       </c>
       <c r="L5" s="55">
-        <f>_xll.xllBlackVolOffSurface(D5,N5,G5,O5,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D5,N5,G5,O5,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.30757466920776261</v>
       </c>
       <c r="M5" s="35">
@@ -6239,7 +6246,7 @@
         <v>0.31757466920776262</v>
       </c>
       <c r="N5" s="36">
-        <f>_xll.xllInterpolate(C5,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C5,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O5" s="51">
@@ -6251,7 +6258,7 @@
         <v>222</v>
       </c>
       <c r="Q5" s="56">
-        <f>_xll.xllInterpolate(P5,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P5,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R5" s="56">
@@ -6259,7 +6266,7 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S5" s="38">
-        <f>_xll.xllBlack(D5,N5,G5,O5,M5*SQRT(O5/365),1)*H5</f>
+        <f>_xll.Black(D5,N5,G5,O5,M5*SQRT(O5/365),1)*H5</f>
         <v>28342.972314952971</v>
       </c>
       <c r="T5" s="57">
@@ -6307,11 +6314,11 @@
         <v>29923.712566763119</v>
       </c>
       <c r="K6" s="55">
-        <f>_xll.xllBlackDelta(D6,N6,G6,O6,M6*SQRT(O6/365),1)</f>
+        <f>_xll.BlackDelta(D6,N6,G6,O6,M6*SQRT(O6/365),1)</f>
         <v>-0.30582858935894086</v>
       </c>
       <c r="L6" s="55">
-        <f>_xll.xllBlackVolOffSurface(D6,N6,G6,O6,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D6,N6,G6,O6,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.2997121519969963</v>
       </c>
       <c r="M6" s="35">
@@ -6319,7 +6326,7 @@
         <v>0.30971215199699631</v>
       </c>
       <c r="N6" s="36">
-        <f>_xll.xllInterpolate(C6,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C6,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O6" s="51">
@@ -6331,7 +6338,7 @@
         <v>252</v>
       </c>
       <c r="Q6" s="56">
-        <f>_xll.xllInterpolate(P6,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P6,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R6" s="56">
@@ -6339,7 +6346,7 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S6" s="38">
-        <f>_xll.xllBlack(D6,N6,G6,O6,M6*SQRT(O6/365),1)*H6</f>
+        <f>_xll.Black(D6,N6,G6,O6,M6*SQRT(O6/365),1)*H6</f>
         <v>30193.679983912178</v>
       </c>
       <c r="T6" s="57">
@@ -6384,11 +6391,11 @@
         <v>31569.634956028829</v>
       </c>
       <c r="K7" s="55">
-        <f>_xll.xllBlackDelta(D7,N7,G7,O7,M7*SQRT(O7/365),1)</f>
+        <f>_xll.BlackDelta(D7,N7,G7,O7,M7*SQRT(O7/365),1)</f>
         <v>-0.30928030961832054</v>
       </c>
       <c r="L7" s="55">
-        <f>_xll.xllBlackVolOffSurface(D7,N7,G7,O7,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D7,N7,G7,O7,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.29359052557809928</v>
       </c>
       <c r="M7" s="35">
@@ -6396,7 +6403,7 @@
         <v>0.30359052557809929</v>
       </c>
       <c r="N7" s="36">
-        <f>_xll.xllInterpolate(C7,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C7,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O7" s="51">
@@ -6408,7 +6415,7 @@
         <v>281</v>
       </c>
       <c r="Q7" s="56">
-        <f>_xll.xllInterpolate(P7,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P7,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R7" s="56">
@@ -6416,7 +6423,7 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S7" s="38">
-        <f>_xll.xllBlack(D7,N7,G7,O7,M7*SQRT(O7/365),1)*H7</f>
+        <f>_xll.Black(D7,N7,G7,O7,M7*SQRT(O7/365),1)*H7</f>
         <v>31893.115812690881</v>
       </c>
       <c r="T7" s="57">
@@ -6460,11 +6467,11 @@
         <v>35516.766330417231</v>
       </c>
       <c r="K8" s="34">
-        <f>_xll.xllBlackDelta(D8,N8,G8,O8,M8*SQRT(O8/365),1)</f>
+        <f>_xll.BlackDelta(D8,N8,G8,O8,M8*SQRT(O8/365),1)</f>
         <v>-0.31688906422406737</v>
       </c>
       <c r="L8" s="34">
-        <f>_xll.xllBlackVolOffSurface(D8,N8,G8,O8,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D8,N8,G8,O8,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28835534081549791</v>
       </c>
       <c r="M8" s="35">
@@ -6472,7 +6479,7 @@
         <v>0.30835534081549792</v>
       </c>
       <c r="N8" s="36">
-        <f>_xll.xllInterpolate(C8,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C8,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O8" s="31">
@@ -6484,7 +6491,7 @@
         <v>314</v>
       </c>
       <c r="Q8" s="37">
-        <f>_xll.xllInterpolate(P8,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P8,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R8" s="37">
@@ -6492,7 +6499,7 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S8" s="38">
-        <f>_xll.xllBlack(D8,N8,G8,O8,M8*SQRT(O8/365),1)*H8</f>
+        <f>_xll.Black(D8,N8,G8,O8,M8*SQRT(O8/365),1)*H8</f>
         <v>35931.407967080631</v>
       </c>
       <c r="T8" s="39">
@@ -6540,11 +6547,11 @@
         <v>37267.211921408147</v>
       </c>
       <c r="K9" s="34">
-        <f>_xll.xllBlackDelta(D9,N9,G9,O9,M9*SQRT(O9/365),1)</f>
+        <f>_xll.BlackDelta(D9,N9,G9,O9,M9*SQRT(O9/365),1)</f>
         <v>-0.31989322539653475</v>
       </c>
       <c r="L9" s="34">
-        <f>_xll.xllBlackVolOffSurface(D9,N9,G9,O9,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D9,N9,G9,O9,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28455903816319966</v>
       </c>
       <c r="M9" s="35">
@@ -6552,7 +6559,7 @@
         <v>0.30455903816319968</v>
       </c>
       <c r="N9" s="36">
-        <f>_xll.xllInterpolate(C9,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C9,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O9" s="31">
@@ -6564,7 +6571,7 @@
         <v>342</v>
       </c>
       <c r="Q9" s="37">
-        <f>_xll.xllInterpolate(P9,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P9,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R9" s="37">
@@ -6572,7 +6579,7 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S9" s="38">
-        <f>_xll.xllBlack(D9,N9,G9,O9,M9*SQRT(O9/365),1)*H9</f>
+        <f>_xll.Black(D9,N9,G9,O9,M9*SQRT(O9/365),1)*H9</f>
         <v>37748.838557378156</v>
       </c>
       <c r="T9" s="39">
@@ -6616,11 +6623,11 @@
         <v>38939.314063721322</v>
       </c>
       <c r="K10" s="34">
-        <f>_xll.xllBlackDelta(D10,N10,G10,O10,M10*SQRT(O10/365),1)</f>
+        <f>_xll.BlackDelta(D10,N10,G10,O10,M10*SQRT(O10/365),1)</f>
         <v>-0.32275039161764552</v>
       </c>
       <c r="L10" s="34">
-        <f>_xll.xllBlackVolOffSurface(D10,N10,G10,O10,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D10,N10,G10,O10,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28058971047977793</v>
       </c>
       <c r="M10" s="35">
@@ -6628,7 +6635,7 @@
         <v>0.30058971047977795</v>
       </c>
       <c r="N10" s="36">
-        <f>_xll.xllInterpolate(C10,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C10,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O10" s="31">
@@ -6640,7 +6647,7 @@
         <v>372</v>
       </c>
       <c r="Q10" s="37">
-        <f>_xll.xllInterpolate(P10,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P10,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R10" s="37">
@@ -6648,7 +6655,7 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S10" s="38">
-        <f>_xll.xllBlack(D10,N10,G10,O10,M10*SQRT(O10/365),1)*H10</f>
+        <f>_xll.Black(D10,N10,G10,O10,M10*SQRT(O10/365),1)*H10</f>
         <v>39496.073908279497</v>
       </c>
       <c r="T10" s="39">
@@ -6693,11 +6700,11 @@
         <v>42084.301804314076</v>
       </c>
       <c r="K11" s="55">
-        <f>_xll.xllBlackDelta(D11,N11,G11,O11,M11*SQRT(O11/365),1)</f>
+        <f>_xll.BlackDelta(D11,N11,G11,O11,M11*SQRT(O11/365),1)</f>
         <v>-0.3279804101698518</v>
       </c>
       <c r="L11" s="55">
-        <f>_xll.xllBlackVolOffSurface(D11,N11,G11,O11,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D11,N11,G11,O11,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27767987513460557</v>
       </c>
       <c r="M11" s="35">
@@ -6705,7 +6712,7 @@
         <v>0.30267987513460559</v>
       </c>
       <c r="N11" s="36">
-        <f>_xll.xllInterpolate(C11,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C11,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O11" s="51">
@@ -6717,7 +6724,7 @@
         <v>403</v>
       </c>
       <c r="Q11" s="56">
-        <f>_xll.xllInterpolate(P11,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P11,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R11" s="56">
@@ -6725,7 +6732,7 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S11" s="38">
-        <f>_xll.xllBlack(D11,N11,G11,O11,M11*SQRT(O11/365),1)*H11</f>
+        <f>_xll.Black(D11,N11,G11,O11,M11*SQRT(O11/365),1)*H11</f>
         <v>42746.671156957244</v>
       </c>
       <c r="T11" s="57">
@@ -6773,11 +6780,11 @@
         <v>43878.267323519292</v>
       </c>
       <c r="K12" s="55">
-        <f>_xll.xllBlackDelta(D12,N12,G12,O12,M12*SQRT(O12/365),1)</f>
+        <f>_xll.BlackDelta(D12,N12,G12,O12,M12*SQRT(O12/365),1)</f>
         <v>-0.33031268997619689</v>
       </c>
       <c r="L12" s="55">
-        <f>_xll.xllBlackVolOffSurface(D12,N12,G12,O12,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D12,N12,G12,O12,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27486507531972315</v>
       </c>
       <c r="M12" s="35">
@@ -6785,7 +6792,7 @@
         <v>0.29986507531972317</v>
       </c>
       <c r="N12" s="36">
-        <f>_xll.xllInterpolate(C12,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C12,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O12" s="51">
@@ -6797,7 +6804,7 @@
         <v>434</v>
       </c>
       <c r="Q12" s="56">
-        <f>_xll.xllInterpolate(P12,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P12,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R12" s="56">
@@ -6805,7 +6812,7 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S12" s="38">
-        <f>_xll.xllBlack(D12,N12,G12,O12,M12*SQRT(O12/365),1)*H12</f>
+        <f>_xll.Black(D12,N12,G12,O12,M12*SQRT(O12/365),1)*H12</f>
         <v>44633.811022245347</v>
       </c>
       <c r="T12" s="57">
@@ -6850,11 +6857,11 @@
         <v>45537.309813921085</v>
       </c>
       <c r="K13" s="55">
-        <f>_xll.xllBlackDelta(D13,N13,G13,O13,M13*SQRT(O13/365),1)</f>
+        <f>_xll.BlackDelta(D13,N13,G13,O13,M13*SQRT(O13/365),1)</f>
         <v>-0.33254501125760916</v>
       </c>
       <c r="L13" s="55">
-        <f>_xll.xllBlackVolOffSurface(D13,N13,G13,O13,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D13,N13,G13,O13,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27247311737224561</v>
       </c>
       <c r="M13" s="35">
@@ -6862,7 +6869,7 @@
         <v>0.29747311737224563</v>
       </c>
       <c r="N13" s="36">
-        <f>_xll.xllInterpolate(C13,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C13,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O13" s="51">
@@ -6874,7 +6881,7 @@
         <v>463</v>
       </c>
       <c r="Q13" s="56">
-        <f>_xll.xllInterpolate(P13,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P13,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R13" s="56">
@@ -6882,7 +6889,7 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S13" s="38">
-        <f>_xll.xllBlack(D13,N13,G13,O13,M13*SQRT(O13/365),1)*H13</f>
+        <f>_xll.Black(D13,N13,G13,O13,M13*SQRT(O13/365),1)*H13</f>
         <v>46386.091242449511</v>
       </c>
       <c r="T13" s="57">
@@ -6922,11 +6929,11 @@
         <v>24164.88926067881</v>
       </c>
       <c r="K15" s="34">
-        <f>_xll.xllBlackDelta(D15,N15,G15,O15,M15*SQRT(O15/365),1)</f>
+        <f>_xll.BlackDelta(D15,N15,G15,O15,M15*SQRT(O15/365),1)</f>
         <v>-0.34573797134889972</v>
       </c>
       <c r="L15" s="34">
-        <f>_xll.xllBlackVolOffSurface(D15,N15,G15,O15,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D15,N15,G15,O15,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.3086688231518766</v>
       </c>
       <c r="M15" s="35">
@@ -6934,7 +6941,7 @@
         <v>0.3086688231518766</v>
       </c>
       <c r="N15" s="36">
-        <f>_xll.xllInterpolate(C15,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C15,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O15" s="31">
@@ -6946,7 +6953,7 @@
         <v>130</v>
       </c>
       <c r="Q15" s="37">
-        <f>_xll.xllInterpolate(P15,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P15,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R15" s="37">
@@ -6954,7 +6961,7 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S15" s="38">
-        <f>_xll.xllBlack(D15,N15,G15,O15,M15*SQRT(O15/365),1)*H15</f>
+        <f>_xll.Black(D15,N15,G15,O15,M15*SQRT(O15/365),1)*H15</f>
         <v>24268.377934815428</v>
       </c>
       <c r="T15" s="39">
@@ -7002,11 +7009,11 @@
         <v>27857.861311981327</v>
       </c>
       <c r="K16" s="34">
-        <f>_xll.xllBlackDelta(D16,N16,G16,O16,M16*SQRT(O16/365),1)</f>
+        <f>_xll.BlackDelta(D16,N16,G16,O16,M16*SQRT(O16/365),1)</f>
         <v>-0.35141008466071144</v>
       </c>
       <c r="L16" s="34">
-        <f>_xll.xllBlackVolOffSurface(D16,N16,G16,O16,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D16,N16,G16,O16,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.30695635331106219</v>
       </c>
       <c r="M16" s="35">
@@ -7014,7 +7021,7 @@
         <v>0.30695635331106219</v>
       </c>
       <c r="N16" s="36">
-        <f>_xll.xllInterpolate(C16,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C16,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O16" s="31">
@@ -7026,7 +7033,7 @@
         <v>161</v>
       </c>
       <c r="Q16" s="37">
-        <f>_xll.xllInterpolate(P16,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P16,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R16" s="37">
@@ -7034,7 +7041,7 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S16" s="38">
-        <f>_xll.xllBlack(D16,N16,G16,O16,M16*SQRT(O16/365),1)*H16</f>
+        <f>_xll.Black(D16,N16,G16,O16,M16*SQRT(O16/365),1)*H16</f>
         <v>28008.951572358888</v>
       </c>
       <c r="T16" s="39">
@@ -7078,11 +7085,11 @@
         <v>30809.684367110713</v>
       </c>
       <c r="K17" s="34">
-        <f>_xll.xllBlackDelta(D17,N17,G17,O17,M17*SQRT(O17/365),1)</f>
+        <f>_xll.BlackDelta(D17,N17,G17,O17,M17*SQRT(O17/365),1)</f>
         <v>-0.35546532307734779</v>
       </c>
       <c r="L17" s="34">
-        <f>_xll.xllBlackVolOffSurface(D17,N17,G17,O17,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D17,N17,G17,O17,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.30365346769227924</v>
       </c>
       <c r="M17" s="35">
@@ -7090,7 +7097,7 @@
         <v>0.30365346769227924</v>
       </c>
       <c r="N17" s="36">
-        <f>_xll.xllInterpolate(C17,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C17,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O17" s="31">
@@ -7102,7 +7109,7 @@
         <v>190</v>
       </c>
       <c r="Q17" s="37">
-        <f>_xll.xllInterpolate(P17,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P17,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R17" s="37">
@@ -7110,7 +7117,7 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S17" s="38">
-        <f>_xll.xllBlack(D17,N17,G17,O17,M17*SQRT(O17/365),1)*H17</f>
+        <f>_xll.Black(D17,N17,G17,O17,M17*SQRT(O17/365),1)*H17</f>
         <v>31010.943189699381</v>
       </c>
       <c r="T17" s="39">
@@ -7155,11 +7162,11 @@
         <v>35542.670900299279</v>
       </c>
       <c r="K18" s="55">
-        <f>_xll.xllBlackDelta(D18,N18,G18,O18,M18*SQRT(O18/365),1)</f>
+        <f>_xll.BlackDelta(D18,N18,G18,O18,M18*SQRT(O18/365),1)</f>
         <v>-0.36196426169418083</v>
       </c>
       <c r="L18" s="55">
-        <f>_xll.xllBlackVolOffSurface(D18,N18,G18,O18,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D18,N18,G18,O18,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.30089879007099096</v>
       </c>
       <c r="M18" s="35">
@@ -7167,7 +7174,7 @@
         <v>0.31089879007099097</v>
       </c>
       <c r="N18" s="36">
-        <f>_xll.xllInterpolate(C18,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C18,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O18" s="51">
@@ -7179,7 +7186,7 @@
         <v>222</v>
       </c>
       <c r="Q18" s="56">
-        <f>_xll.xllInterpolate(P18,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P18,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R18" s="56">
@@ -7187,7 +7194,7 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S18" s="38">
-        <f>_xll.xllBlack(D18,N18,G18,O18,M18*SQRT(O18/365),1)*H18</f>
+        <f>_xll.Black(D18,N18,G18,O18,M18*SQRT(O18/365),1)*H18</f>
         <v>35819.729225762312</v>
       </c>
       <c r="T18" s="57">
@@ -7235,11 +7242,11 @@
         <v>37524.648723895007</v>
       </c>
       <c r="K19" s="55">
-        <f>_xll.xllBlackDelta(D19,N19,G19,O19,M19*SQRT(O19/365),1)</f>
+        <f>_xll.BlackDelta(D19,N19,G19,O19,M19*SQRT(O19/365),1)</f>
         <v>-0.36366372008794157</v>
       </c>
       <c r="L19" s="55">
-        <f>_xll.xllBlackVolOffSurface(D19,N19,G19,O19,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D19,N19,G19,O19,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.29381889318776599</v>
       </c>
       <c r="M19" s="35">
@@ -7247,7 +7254,7 @@
         <v>0.303818893187766</v>
       </c>
       <c r="N19" s="36">
-        <f>_xll.xllInterpolate(C19,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C19,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O19" s="51">
@@ -7259,7 +7266,7 @@
         <v>252</v>
       </c>
       <c r="Q19" s="56">
-        <f>_xll.xllInterpolate(P19,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P19,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R19" s="56">
@@ -7267,7 +7274,7 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S19" s="38">
-        <f>_xll.xllBlack(D19,N19,G19,O19,M19*SQRT(O19/365),1)*H19</f>
+        <f>_xll.Black(D19,N19,G19,O19,M19*SQRT(O19/365),1)*H19</f>
         <v>37863.190690330943</v>
       </c>
       <c r="T19" s="57">
@@ -7312,11 +7319,11 @@
         <v>39306.477392963388</v>
       </c>
       <c r="K20" s="55">
-        <f>_xll.xllBlackDelta(D20,N20,G20,O20,M20*SQRT(O20/365),1)</f>
+        <f>_xll.BlackDelta(D20,N20,G20,O20,M20*SQRT(O20/365),1)</f>
         <v>-0.36545488048703523</v>
       </c>
       <c r="L20" s="55">
-        <f>_xll.xllBlackVolOffSurface(D20,N20,G20,O20,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D20,N20,G20,O20,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28813992233363023</v>
       </c>
       <c r="M20" s="35">
@@ -7324,7 +7331,7 @@
         <v>0.29813992233363024</v>
       </c>
       <c r="N20" s="36">
-        <f>_xll.xllInterpolate(C20,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C20,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O20" s="51">
@@ -7336,7 +7343,7 @@
         <v>281</v>
       </c>
       <c r="Q20" s="56">
-        <f>_xll.xllInterpolate(P20,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P20,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R20" s="56">
@@ -7344,7 +7351,7 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S20" s="38">
-        <f>_xll.xllBlack(D20,N20,G20,O20,M20*SQRT(O20/365),1)*H20</f>
+        <f>_xll.Black(D20,N20,G20,O20,M20*SQRT(O20/365),1)*H20</f>
         <v>39709.234440903703</v>
       </c>
       <c r="T20" s="57">
@@ -7388,11 +7395,11 @@
         <v>43548.734377815155</v>
       </c>
       <c r="K21" s="34">
-        <f>_xll.xllBlackDelta(D21,N21,G21,O21,M21*SQRT(O21/365),1)</f>
+        <f>_xll.BlackDelta(D21,N21,G21,O21,M21*SQRT(O21/365),1)</f>
         <v>-0.36959975330397976</v>
       </c>
       <c r="L21" s="34">
-        <f>_xll.xllBlackVolOffSurface(D21,N21,G21,O21,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D21,N21,G21,O21,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28336120771860407</v>
       </c>
       <c r="M21" s="35">
@@ -7400,7 +7407,7 @@
         <v>0.30336120771860409</v>
       </c>
       <c r="N21" s="36">
-        <f>_xll.xllInterpolate(C21,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C21,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O21" s="31">
@@ -7412,7 +7419,7 @@
         <v>314</v>
       </c>
       <c r="Q21" s="37">
-        <f>_xll.xllInterpolate(P21,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P21,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R21" s="37">
@@ -7420,7 +7427,7 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S21" s="38">
-        <f>_xll.xllBlack(D21,N21,G21,O21,M21*SQRT(O21/365),1)*H21</f>
+        <f>_xll.Black(D21,N21,G21,O21,M21*SQRT(O21/365),1)*H21</f>
         <v>44057.145485094719</v>
       </c>
       <c r="T21" s="39">
@@ -7468,11 +7475,11 @@
         <v>45432.896545259384</v>
       </c>
       <c r="K22" s="34">
-        <f>_xll.xllBlackDelta(D22,N22,G22,O22,M22*SQRT(O22/365),1)</f>
+        <f>_xll.BlackDelta(D22,N22,G22,O22,M22*SQRT(O22/365),1)</f>
         <v>-0.37119693825929057</v>
       </c>
       <c r="L22" s="34">
-        <f>_xll.xllBlackVolOffSurface(D22,N22,G22,O22,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D22,N22,G22,O22,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27991423340969296</v>
       </c>
       <c r="M22" s="35">
@@ -7480,7 +7487,7 @@
         <v>0.29991423340969298</v>
       </c>
       <c r="N22" s="36">
-        <f>_xll.xllInterpolate(C22,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C22,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O22" s="31">
@@ -7492,7 +7499,7 @@
         <v>342</v>
       </c>
       <c r="Q22" s="37">
-        <f>_xll.xllInterpolate(P22,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P22,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R22" s="37">
@@ -7500,7 +7507,7 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S22" s="38">
-        <f>_xll.xllBlack(D22,N22,G22,O22,M22*SQRT(O22/365),1)*H22</f>
+        <f>_xll.Black(D22,N22,G22,O22,M22*SQRT(O22/365),1)*H22</f>
         <v>46020.053244065086</v>
       </c>
       <c r="T22" s="39">
@@ -7544,11 +7551,11 @@
         <v>47239.376020054093</v>
       </c>
       <c r="K23" s="34">
-        <f>_xll.xllBlackDelta(D23,N23,G23,O23,M23*SQRT(O23/365),1)</f>
+        <f>_xll.BlackDelta(D23,N23,G23,O23,M23*SQRT(O23/365),1)</f>
         <v>-0.37281579543426202</v>
       </c>
       <c r="L23" s="34">
-        <f>_xll.xllBlackVolOffSurface(D23,N23,G23,O23,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D23,N23,G23,O23,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27630259244482691</v>
       </c>
       <c r="M23" s="35">
@@ -7556,7 +7563,7 @@
         <v>0.29630259244482693</v>
       </c>
       <c r="N23" s="36">
-        <f>_xll.xllInterpolate(C23,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C23,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O23" s="31">
@@ -7568,7 +7575,7 @@
         <v>372</v>
       </c>
       <c r="Q23" s="37">
-        <f>_xll.xllInterpolate(P23,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P23,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R23" s="37">
@@ -7576,7 +7583,7 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S23" s="38">
-        <f>_xll.xllBlack(D23,N23,G23,O23,M23*SQRT(O23/365),1)*H23</f>
+        <f>_xll.Black(D23,N23,G23,O23,M23*SQRT(O23/365),1)*H23</f>
         <v>47914.811329646625</v>
       </c>
       <c r="T23" s="39">
@@ -7621,11 +7628,11 @@
         <v>50609.824972630813</v>
       </c>
       <c r="K24" s="55">
-        <f>_xll.xllBlackDelta(D24,N24,G24,O24,M24*SQRT(O24/365),1)</f>
+        <f>_xll.BlackDelta(D24,N24,G24,O24,M24*SQRT(O24/365),1)</f>
         <v>-0.37598158235809376</v>
       </c>
       <c r="L24" s="55">
-        <f>_xll.xllBlackVolOffSurface(D24,N24,G24,O24,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D24,N24,G24,O24,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27372331879253742</v>
       </c>
       <c r="M24" s="35">
@@ -7633,7 +7640,7 @@
         <v>0.29872331879253744</v>
       </c>
       <c r="N24" s="36">
-        <f>_xll.xllInterpolate(C24,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C24,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O24" s="51">
@@ -7645,7 +7652,7 @@
         <v>403</v>
       </c>
       <c r="Q24" s="56">
-        <f>_xll.xllInterpolate(P24,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P24,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R24" s="56">
@@ -7653,7 +7660,7 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S24" s="38">
-        <f>_xll.xllBlack(D24,N24,G24,O24,M24*SQRT(O24/365),1)*H24</f>
+        <f>_xll.Black(D24,N24,G24,O24,M24*SQRT(O24/365),1)*H24</f>
         <v>51406.378451416793</v>
       </c>
       <c r="T24" s="57">
@@ -7701,11 +7708,11 @@
         <v>52512.817255302056</v>
       </c>
       <c r="K25" s="55">
-        <f>_xll.xllBlackDelta(D25,N25,G25,O25,M25*SQRT(O25/365),1)</f>
+        <f>_xll.BlackDelta(D25,N25,G25,O25,M25*SQRT(O25/365),1)</f>
         <v>-0.37711344566546012</v>
       </c>
       <c r="L25" s="55">
-        <f>_xll.xllBlackVolOffSurface(D25,N25,G25,O25,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D25,N25,G25,O25,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27112228252390913</v>
       </c>
       <c r="M25" s="35">
@@ -7713,7 +7720,7 @@
         <v>0.29612228252390915</v>
       </c>
       <c r="N25" s="36">
-        <f>_xll.xllInterpolate(C25,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C25,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O25" s="51">
@@ -7725,7 +7732,7 @@
         <v>434</v>
       </c>
       <c r="Q25" s="56">
-        <f>_xll.xllInterpolate(P25,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P25,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R25" s="56">
@@ -7733,7 +7740,7 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S25" s="38">
-        <f>_xll.xllBlack(D25,N25,G25,O25,M25*SQRT(O25/365),1)*H25</f>
+        <f>_xll.Black(D25,N25,G25,O25,M25*SQRT(O25/365),1)*H25</f>
         <v>53417.04001977593</v>
       </c>
       <c r="T25" s="57">
@@ -7778,11 +7785,11 @@
         <v>54284.024997653694</v>
       </c>
       <c r="K26" s="55">
-        <f>_xll.xllBlackDelta(D26,N26,G26,O26,M26*SQRT(O26/365),1)</f>
+        <f>_xll.BlackDelta(D26,N26,G26,O26,M26*SQRT(O26/365),1)</f>
         <v>-0.37832705670325517</v>
       </c>
       <c r="L26" s="55">
-        <f>_xll.xllBlackVolOffSurface(D26,N26,G26,O26,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D26,N26,G26,O26,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.26896241362104312</v>
       </c>
       <c r="M26" s="35">
@@ -7790,7 +7797,7 @@
         <v>0.29396241362104314</v>
       </c>
       <c r="N26" s="36">
-        <f>_xll.xllInterpolate(C26,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C26,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O26" s="51">
@@ -7802,7 +7809,7 @@
         <v>463</v>
       </c>
       <c r="Q26" s="56">
-        <f>_xll.xllInterpolate(P26,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P26,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R26" s="56">
@@ -7810,7 +7817,7 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S26" s="38">
-        <f>_xll.xllBlack(D26,N26,G26,O26,M26*SQRT(O26/365),1)*H26</f>
+        <f>_xll.Black(D26,N26,G26,O26,M26*SQRT(O26/365),1)*H26</f>
         <v>55295.838661483605</v>
       </c>
       <c r="T26" s="57">
@@ -7850,11 +7857,11 @@
         <v>32265.67129512161</v>
       </c>
       <c r="K28" s="34">
-        <f>_xll.xllBlackDelta(D28,N28,G28,O28,M28*SQRT(O28/365),1)</f>
+        <f>_xll.BlackDelta(D28,N28,G28,O28,M28*SQRT(O28/365),1)</f>
         <v>-0.42936085127013446</v>
       </c>
       <c r="L28" s="34">
-        <f>_xll.xllBlackVolOffSurface(D28,N28,G28,O28,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D28,N28,G28,O28,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.30028135827806668</v>
       </c>
       <c r="M28" s="35">
@@ -7862,7 +7869,7 @@
         <v>0.30028135827806668</v>
       </c>
       <c r="N28" s="36">
-        <f>_xll.xllInterpolate(C28,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C28,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.83</v>
       </c>
       <c r="O28" s="31">
@@ -7874,7 +7881,7 @@
         <v>130</v>
       </c>
       <c r="Q28" s="37">
-        <f>_xll.xllInterpolate(P28,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P28,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.19045E-2</v>
       </c>
       <c r="R28" s="37">
@@ -7882,7 +7889,7 @@
         <v>0.99573565755343896</v>
       </c>
       <c r="S28" s="38">
-        <f>_xll.xllBlack(D28,N28,G28,O28,M28*SQRT(O28/365),1)*H28</f>
+        <f>_xll.Black(D28,N28,G28,O28,M28*SQRT(O28/365),1)*H28</f>
         <v>32403.852418421586</v>
       </c>
       <c r="T28" s="39">
@@ -7930,11 +7937,11 @@
         <v>36137.73704002802</v>
       </c>
       <c r="K29" s="34">
-        <f>_xll.xllBlackDelta(D29,N29,G29,O29,M29*SQRT(O29/365),1)</f>
+        <f>_xll.BlackDelta(D29,N29,G29,O29,M29*SQRT(O29/365),1)</f>
         <v>-0.42680978137342407</v>
       </c>
       <c r="L29" s="34">
-        <f>_xll.xllBlackVolOffSurface(D29,N29,G29,O29,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D29,N29,G29,O29,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.29943271260105442</v>
       </c>
       <c r="M29" s="35">
@@ -7942,7 +7949,7 @@
         <v>0.29943271260105442</v>
       </c>
       <c r="N29" s="36">
-        <f>_xll.xllInterpolate(C29,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C29,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.89</v>
       </c>
       <c r="O29" s="31">
@@ -7954,7 +7961,7 @@
         <v>161</v>
       </c>
       <c r="Q29" s="37">
-        <f>_xll.xllInterpolate(P29,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P29,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2168000000000002E-2</v>
       </c>
       <c r="R29" s="37">
@@ -7962,7 +7969,7 @@
         <v>0.99460564384256822</v>
       </c>
       <c r="S29" s="38">
-        <f>_xll.xllBlack(D29,N29,G29,O29,M29*SQRT(O29/365),1)*H29</f>
+        <f>_xll.Black(D29,N29,G29,O29,M29*SQRT(O29/365),1)*H29</f>
         <v>36333.734142522226</v>
       </c>
       <c r="T29" s="39">
@@ -8006,11 +8013,11 @@
         <v>39232.064799529231</v>
       </c>
       <c r="K30" s="34">
-        <f>_xll.xllBlackDelta(D30,N30,G30,O30,M30*SQRT(O30/365),1)</f>
+        <f>_xll.BlackDelta(D30,N30,G30,O30,M30*SQRT(O30/365),1)</f>
         <v>-0.4255852974904103</v>
       </c>
       <c r="L30" s="34">
-        <f>_xll.xllBlackVolOffSurface(D30,N30,G30,O30,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D30,N30,G30,O30,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.29674381144091944</v>
       </c>
       <c r="M30" s="35">
@@ -8018,7 +8025,7 @@
         <v>0.29674381144091944</v>
       </c>
       <c r="N30" s="36">
-        <f>_xll.xllInterpolate(C30,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
+        <f>_xll.Interpolate(C30,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.2</f>
         <v>52.91</v>
       </c>
       <c r="O30" s="31">
@@ -8030,7 +8037,7 @@
         <v>190</v>
       </c>
       <c r="Q30" s="37">
-        <f>_xll.xllInterpolate(P30,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P30,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2413195652173914E-2</v>
       </c>
       <c r="R30" s="37">
@@ -8038,7 +8045,7 @@
         <v>0.99351007090118049</v>
       </c>
       <c r="S30" s="38">
-        <f>_xll.xllBlack(D30,N30,G30,O30,M30*SQRT(O30/365),1)*H30</f>
+        <f>_xll.Black(D30,N30,G30,O30,M30*SQRT(O30/365),1)*H30</f>
         <v>39488.341335023521</v>
       </c>
       <c r="T30" s="39">
@@ -8083,11 +8090,11 @@
         <v>44184.538435842187</v>
       </c>
       <c r="K31" s="55">
-        <f>_xll.xllBlackDelta(D31,N31,G31,O31,M31*SQRT(O31/365),1)</f>
+        <f>_xll.BlackDelta(D31,N31,G31,O31,M31*SQRT(O31/365),1)</f>
         <v>-0.42550473632764729</v>
       </c>
       <c r="L31" s="55">
-        <f>_xll.xllBlackVolOffSurface(D31,N31,G31,O31,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D31,N31,G31,O31,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.29437980749351916</v>
       </c>
       <c r="M31" s="35">
@@ -8095,7 +8102,7 @@
         <v>0.30437980749351917</v>
       </c>
       <c r="N31" s="36">
-        <f>_xll.xllInterpolate(C31,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C31,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O31" s="51">
@@ -8107,7 +8114,7 @@
         <v>222</v>
       </c>
       <c r="Q31" s="56">
-        <f>_xll.xllInterpolate(P31,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P31,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2671282608695654E-2</v>
       </c>
       <c r="R31" s="56">
@@ -8115,7 +8122,7 @@
         <v>0.99226520324269329</v>
       </c>
       <c r="S31" s="38">
-        <f>_xll.xllBlack(D31,N31,G31,O31,M31*SQRT(O31/365),1)*H31</f>
+        <f>_xll.Black(D31,N31,G31,O31,M31*SQRT(O31/365),1)*H31</f>
         <v>44528.960898203848</v>
       </c>
       <c r="T31" s="57">
@@ -8163,11 +8170,11 @@
         <v>46284.700241535189</v>
       </c>
       <c r="K32" s="55">
-        <f>_xll.xllBlackDelta(D32,N32,G32,O32,M32*SQRT(O32/365),1)</f>
+        <f>_xll.BlackDelta(D32,N32,G32,O32,M32*SQRT(O32/365),1)</f>
         <v>-0.42464550509498566</v>
       </c>
       <c r="L32" s="55">
-        <f>_xll.xllBlackVolOffSurface(D32,N32,G32,O32,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D32,N32,G32,O32,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28793908707932159</v>
       </c>
       <c r="M32" s="35">
@@ -8175,7 +8182,7 @@
         <v>0.2979390870793216</v>
       </c>
       <c r="N32" s="36">
-        <f>_xll.xllInterpolate(C32,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C32,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.87</v>
       </c>
       <c r="O32" s="51">
@@ -8187,7 +8194,7 @@
         <v>252</v>
       </c>
       <c r="Q32" s="56">
-        <f>_xll.xllInterpolate(P32,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P32,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.2913239130434784E-2</v>
       </c>
       <c r="R32" s="56">
@@ -8195,7 +8202,7 @@
         <v>0.99105881041022814</v>
       </c>
       <c r="S32" s="38">
-        <f>_xll.xllBlack(D32,N32,G32,O32,M32*SQRT(O32/365),1)*H32</f>
+        <f>_xll.Black(D32,N32,G32,O32,M32*SQRT(O32/365),1)*H32</f>
         <v>46702.274128794234</v>
       </c>
       <c r="T32" s="57">
@@ -8240,11 +8247,11 @@
         <v>48194.988240876482</v>
       </c>
       <c r="K33" s="55">
-        <f>_xll.xllBlackDelta(D33,N33,G33,O33,M33*SQRT(O33/365),1)</f>
+        <f>_xll.BlackDelta(D33,N33,G33,O33,M33*SQRT(O33/365),1)</f>
         <v>-0.42439749124093862</v>
       </c>
       <c r="L33" s="55">
-        <f>_xll.xllBlackVolOffSurface(D33,N33,G33,O33,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D33,N33,G33,O33,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.28286439866994223</v>
       </c>
       <c r="M33" s="35">
@@ -8252,7 +8259,7 @@
         <v>0.29286439866994224</v>
       </c>
       <c r="N33" s="36">
-        <f>_xll.xllInterpolate(C33,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
+        <f>_xll.Interpolate(C33,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.25</f>
         <v>52.850000000000009</v>
       </c>
       <c r="O33" s="51">
@@ -8264,7 +8271,7 @@
         <v>281</v>
       </c>
       <c r="Q33" s="56">
-        <f>_xll.xllInterpolate(P33,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P33,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3146155555555556E-2</v>
       </c>
       <c r="R33" s="56">
@@ -8272,7 +8279,7 @@
         <v>0.98985734543586568</v>
       </c>
       <c r="S33" s="38">
-        <f>_xll.xllBlack(D33,N33,G33,O33,M33*SQRT(O33/365),1)*H33</f>
+        <f>_xll.Black(D33,N33,G33,O33,M33*SQRT(O33/365),1)*H33</f>
         <v>48688.822145028076</v>
       </c>
       <c r="T33" s="57">
@@ -8316,11 +8323,11 @@
         <v>52661.669155425981</v>
       </c>
       <c r="K34" s="34">
-        <f>_xll.xllBlackDelta(D34,N34,G34,O34,M34*SQRT(O34/365),1)</f>
+        <f>_xll.BlackDelta(D34,N34,G34,O34,M34*SQRT(O34/365),1)</f>
         <v>-0.42442357038188716</v>
       </c>
       <c r="L34" s="34">
-        <f>_xll.xllBlackVolOffSurface(D34,N34,G34,O34,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D34,N34,G34,O34,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27855979919652529</v>
       </c>
       <c r="M34" s="35">
@@ -8328,7 +8335,7 @@
         <v>0.29855979919652531</v>
       </c>
       <c r="N34" s="36">
-        <f>_xll.xllInterpolate(C34,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C34,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.77</v>
       </c>
       <c r="O34" s="31">
@@ -8340,7 +8347,7 @@
         <v>314</v>
       </c>
       <c r="Q34" s="37">
-        <f>_xll.xllInterpolate(P34,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P34,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3396222222222223E-2</v>
       </c>
       <c r="R34" s="37">
@@ -8348,7 +8355,7 @@
         <v>0.98846018956331227</v>
       </c>
       <c r="S34" s="38">
-        <f>_xll.xllBlack(D34,N34,G34,O34,M34*SQRT(O34/365),1)*H34</f>
+        <f>_xll.Black(D34,N34,G34,O34,M34*SQRT(O34/365),1)*H34</f>
         <v>53276.469514357639</v>
       </c>
       <c r="T34" s="39">
@@ -8396,11 +8403,11 @@
         <v>54652.425754458432</v>
       </c>
       <c r="K35" s="34">
-        <f>_xll.xllBlackDelta(D35,N35,G35,O35,M35*SQRT(O35/365),1)</f>
+        <f>_xll.BlackDelta(D35,N35,G35,O35,M35*SQRT(O35/365),1)</f>
         <v>-0.42434781074794536</v>
       </c>
       <c r="L35" s="34">
-        <f>_xll.xllBlackVolOffSurface(D35,N35,G35,O35,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D35,N35,G35,O35,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.27547069125621454</v>
       </c>
       <c r="M35" s="35">
@@ -8408,7 +8415,7 @@
         <v>0.29547069125621456</v>
       </c>
       <c r="N35" s="36">
-        <f>_xll.xllInterpolate(C35,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C35,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.730000000000004</v>
       </c>
       <c r="O35" s="31">
@@ -8420,7 +8427,7 @@
         <v>342</v>
       </c>
       <c r="Q35" s="37">
-        <f>_xll.xllInterpolate(P35,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P35,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.36084E-2</v>
       </c>
       <c r="R35" s="37">
@@ -8428,7 +8435,7 @@
         <v>0.98724128597392646</v>
       </c>
       <c r="S35" s="38">
-        <f>_xll.xllBlack(D35,N35,G35,O35,M35*SQRT(O35/365),1)*H35</f>
+        <f>_xll.Black(D35,N35,G35,O35,M35*SQRT(O35/365),1)*H35</f>
         <v>55358.731984697231</v>
       </c>
       <c r="T35" s="39">
@@ -8472,11 +8479,11 @@
         <v>56554.27385336806</v>
       </c>
       <c r="K36" s="34">
-        <f>_xll.xllBlackDelta(D36,N36,G36,O36,M36*SQRT(O36/365),1)</f>
+        <f>_xll.BlackDelta(D36,N36,G36,O36,M36*SQRT(O36/365),1)</f>
         <v>-0.42449567535457533</v>
       </c>
       <c r="L36" s="34">
-        <f>_xll.xllBlackVolOffSurface(D36,N36,G36,O36,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D36,N36,G36,O36,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.2721468149249171</v>
       </c>
       <c r="M36" s="35">
@@ -8484,7 +8491,7 @@
         <v>0.29214681492491712</v>
       </c>
       <c r="N36" s="36">
-        <f>_xll.xllInterpolate(C36,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
+        <f>_xll.Interpolate(C36,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.3</f>
         <v>52.680000000000007</v>
       </c>
       <c r="O36" s="31">
@@ -8496,7 +8503,7 @@
         <v>372</v>
       </c>
       <c r="Q36" s="37">
-        <f>_xll.xllInterpolate(P36,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P36,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.3833736263736263E-2</v>
       </c>
       <c r="R36" s="37">
@@ -8504,7 +8511,7 @@
         <v>0.98590341293539407</v>
       </c>
       <c r="S36" s="38">
-        <f>_xll.xllBlack(D36,N36,G36,O36,M36*SQRT(O36/365),1)*H36</f>
+        <f>_xll.Black(D36,N36,G36,O36,M36*SQRT(O36/365),1)*H36</f>
         <v>57362.894895540892</v>
       </c>
       <c r="T36" s="39">
@@ -8549,11 +8556,11 @@
         <v>60086.280429461578</v>
       </c>
       <c r="K37" s="55">
-        <f>_xll.xllBlackDelta(D37,N37,G37,O37,M37*SQRT(O37/365),1)</f>
+        <f>_xll.BlackDelta(D37,N37,G37,O37,M37*SQRT(O37/365),1)</f>
         <v>-0.42527466628415733</v>
       </c>
       <c r="L37" s="55">
-        <f>_xll.xllBlackVolOffSurface(D37,N37,G37,O37,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D37,N37,G37,O37,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.26980378002809019</v>
       </c>
       <c r="M37" s="35">
@@ -8561,7 +8568,7 @@
         <v>0.29480378002809021</v>
       </c>
       <c r="N37" s="36">
-        <f>_xll.xllInterpolate(C37,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C37,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.559999999999995</v>
       </c>
       <c r="O37" s="51">
@@ -8573,7 +8580,7 @@
         <v>403</v>
       </c>
       <c r="Q37" s="56">
-        <f>_xll.xllInterpolate(P37,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P37,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4048010989010989E-2</v>
       </c>
       <c r="R37" s="56">
@@ -8581,7 +8588,7 @@
         <v>0.98450477347789078</v>
       </c>
       <c r="S37" s="38">
-        <f>_xll.xllBlack(D37,N37,G37,O37,M37*SQRT(O37/365),1)*H37</f>
+        <f>_xll.Black(D37,N37,G37,O37,M37*SQRT(O37/365),1)*H37</f>
         <v>61031.984859960605</v>
       </c>
       <c r="T37" s="57">
@@ -8629,11 +8636,11 @@
         <v>62098.511986835096</v>
       </c>
       <c r="K38" s="55">
-        <f>_xll.xllBlackDelta(D38,N38,G38,O38,M38*SQRT(O38/365),1)</f>
+        <f>_xll.BlackDelta(D38,N38,G38,O38,M38*SQRT(O38/365),1)</f>
         <v>-0.42502667104308745</v>
       </c>
       <c r="L38" s="55">
-        <f>_xll.xllBlackVolOffSurface(D38,N38,G38,O38,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D38,N38,G38,O38,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.26753735396207162</v>
       </c>
       <c r="M38" s="35">
@@ -8641,7 +8648,7 @@
         <v>0.29253735396207164</v>
       </c>
       <c r="N38" s="36">
-        <f>_xll.xllInterpolate(C38,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C38,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.51</v>
       </c>
       <c r="O38" s="51">
@@ -8653,7 +8660,7 @@
         <v>434</v>
       </c>
       <c r="Q38" s="56">
-        <f>_xll.xllInterpolate(P38,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P38,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4262285714285713E-2</v>
       </c>
       <c r="R38" s="56">
@@ -8661,7 +8668,7 @@
         <v>0.98307239105463129</v>
       </c>
       <c r="S38" s="38">
-        <f>_xll.xllBlack(D38,N38,G38,O38,M38*SQRT(O38/365),1)*H38</f>
+        <f>_xll.Black(D38,N38,G38,O38,M38*SQRT(O38/365),1)*H38</f>
         <v>63167.791662032505</v>
       </c>
       <c r="T38" s="57">
@@ -8706,11 +8713,11 @@
         <v>63946.931178454251</v>
       </c>
       <c r="K39" s="55">
-        <f>_xll.xllBlackDelta(D39,N39,G39,O39,M39*SQRT(O39/365),1)</f>
+        <f>_xll.BlackDelta(D39,N39,G39,O39,M39*SQRT(O39/365),1)</f>
         <v>-0.42508194233890251</v>
       </c>
       <c r="L39" s="55">
-        <f>_xll.xllBlackVolOffSurface(D39,N39,G39,O39,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
+        <f>_xll.BlackVolOffSurface(D39,N39,G39,O39,'LCO Vol Surf'!$S$2:$S$29,'LCO Vol Surf'!$B$30:$R$30,'LCO Vol Surf'!$B$2:$R$29,$L$1)</f>
         <v>0.26554751559010453</v>
       </c>
       <c r="M39" s="35">
@@ -8718,7 +8725,7 @@
         <v>0.29054751559010455</v>
       </c>
       <c r="N39" s="36">
-        <f>_xll.xllInterpolate(C39,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
+        <f>_xll.Interpolate(C39,Rates!$D$4:$D$36,Rates!$E$4:$E$36,COUNT(Rates!$D$4:$D$36))-0.35</f>
         <v>52.449999999999982</v>
       </c>
       <c r="O39" s="51">
@@ -8730,7 +8737,7 @@
         <v>463</v>
       </c>
       <c r="Q39" s="56">
-        <f>_xll.xllInterpolate(P39,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
+        <f>_xll.Interpolate(P39,Rates!$A$4:$A$54,Rates!$B$4:$B$54,Rates!$A$2)/100</f>
         <v>1.4462902173913045E-2</v>
       </c>
       <c r="R39" s="56">
@@ -8738,7 +8745,7 @@
         <v>0.98170181177603344</v>
       </c>
       <c r="S39" s="38">
-        <f>_xll.xllBlack(D39,N39,G39,O39,M39*SQRT(O39/365),1)*H39</f>
+        <f>_xll.Black(D39,N39,G39,O39,M39*SQRT(O39/365),1)*H39</f>
         <v>65138.854193174469</v>
       </c>
       <c r="T39" s="57">

</xml_diff>